<commit_message>
Update external data 2017
</commit_message>
<xml_diff>
--- a/data-input/wb-data/global-economic-monitor/Emerging Market Bond Index (JPM Total Return Index).xlsx
+++ b/data-input/wb-data/global-economic-monitor/Emerging Market Bond Index (JPM Total Return Index).xlsx
@@ -5,14 +5,14 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="annual" sheetId="1" r:id="Rd2c71305527a4999"/>
-    <sheet name="monthly" sheetId="2" r:id="Re0b33552d30e4740"/>
+    <sheet name="annual" sheetId="1" r:id="R0a9f01d49cd04cce"/>
+    <sheet name="monthly" sheetId="2" r:id="R8109e013a1dd4f0c"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="393">
   <si>
     <t/>
   </si>
@@ -1153,6 +1153,45 @@
   <si>
     <t>2017M05</t>
   </si>
+  <si>
+    <t>2017M06</t>
+  </si>
+  <si>
+    <t>2017M07</t>
+  </si>
+  <si>
+    <t>2017M08</t>
+  </si>
+  <si>
+    <t>2017M09</t>
+  </si>
+  <si>
+    <t>2017M10</t>
+  </si>
+  <si>
+    <t>2017M11</t>
+  </si>
+  <si>
+    <t>2017M12</t>
+  </si>
+  <si>
+    <t>2018M01</t>
+  </si>
+  <si>
+    <t>2018M02</t>
+  </si>
+  <si>
+    <t>2018M03</t>
+  </si>
+  <si>
+    <t>2018M04</t>
+  </si>
+  <si>
+    <t>2018M05</t>
+  </si>
+  <si>
+    <t>2018M06</t>
+  </si>
 </sst>
 </file>
 
@@ -1197,7 +1236,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AX30"/>
+  <dimension ref="A1:AX31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5616,151 +5655,303 @@
         <v>2017</v>
       </c>
       <c r="B30" s="0">
-        <v>298.7677</v>
+        <v>312.4403</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>50</v>
+      <c r="D30" s="0">
+        <v>102.5118</v>
       </c>
       <c r="E30" s="0">
-        <v>133.02</v>
+        <v>145.696</v>
       </c>
       <c r="F30" s="0">
-        <v>1110.006</v>
+        <v>1141.895</v>
       </c>
       <c r="G30" s="0">
-        <v>338.0221</v>
+        <v>346.8973</v>
       </c>
       <c r="H30" s="0">
-        <v>467.2907</v>
+        <v>474.5639</v>
       </c>
       <c r="I30" s="0">
-        <v>246.1352</v>
+        <v>257.0055</v>
       </c>
       <c r="J30" s="0">
-        <v>567.5512</v>
+        <v>582.0092</v>
       </c>
       <c r="K30" s="0">
-        <v>765.4304</v>
+        <v>784.5871</v>
       </c>
       <c r="L30" s="0">
-        <v>413.2959</v>
+        <v>431.8997</v>
       </c>
       <c r="M30" s="0">
-        <v>1010.05</v>
+        <v>1051.04</v>
       </c>
       <c r="N30" s="0">
-        <v>307.6356</v>
+        <v>319.1761</v>
       </c>
       <c r="O30" s="0">
-        <v>211.2394</v>
+        <v>218.3362</v>
       </c>
       <c r="P30" s="0">
-        <v>226.2743</v>
+        <v>232.0438</v>
       </c>
       <c r="Q30" s="0">
-        <v>231.5121</v>
+        <v>246.6009</v>
       </c>
       <c r="R30" s="0">
-        <v>162.4309</v>
+        <v>166.531</v>
       </c>
       <c r="S30" s="0">
-        <v>315.7248</v>
+        <v>323.1576</v>
       </c>
       <c r="T30" s="0">
-        <v>320.244</v>
+        <v>330.0967</v>
       </c>
       <c r="U30" s="0">
-        <v>296.8212</v>
+        <v>314.2443</v>
       </c>
       <c r="V30" s="0">
-        <v>250.2176</v>
+        <v>261.877</v>
       </c>
       <c r="W30" s="0">
-        <v>109.2859</v>
+        <v>112.3001</v>
       </c>
       <c r="X30" s="0">
-        <v>201.0759</v>
+        <v>207.0883</v>
       </c>
       <c r="Y30" s="0">
-        <v>682.7226</v>
+        <v>700.1031</v>
       </c>
       <c r="Z30" s="0">
-        <v>504.0743</v>
+        <v>506.4694</v>
       </c>
       <c r="AA30" s="0">
-        <v>230.012</v>
+        <v>238.1539</v>
       </c>
       <c r="AB30" s="0">
-        <v>176.3506</v>
+        <v>178.8438</v>
       </c>
       <c r="AC30" s="0">
-        <v>125.1186</v>
+        <v>128.8848</v>
       </c>
       <c r="AD30" s="0">
-        <v>648.711</v>
+        <v>673.2803</v>
       </c>
       <c r="AE30" s="0">
-        <v>524.4887</v>
+        <v>531.0272</v>
       </c>
       <c r="AF30" s="0">
-        <v>390.5243</v>
+        <v>398.6465</v>
       </c>
       <c r="AG30" s="0">
-        <v>155.9599</v>
+        <v>162.1726</v>
       </c>
       <c r="AH30" s="0">
-        <v>315.3009</v>
+        <v>320.4919</v>
       </c>
       <c r="AI30" s="0">
-        <v>1317.281</v>
+        <v>1359.7</v>
       </c>
       <c r="AJ30" s="0">
-        <v>1249.478</v>
+        <v>1289.767</v>
       </c>
       <c r="AK30" s="0">
-        <v>838.776</v>
+        <v>853.5987</v>
       </c>
       <c r="AL30" s="0">
-        <v>616.713</v>
+        <v>628.5354</v>
       </c>
       <c r="AM30" s="0">
-        <v>1100.546</v>
+        <v>1116.187</v>
       </c>
       <c r="AN30" s="0">
-        <v>167.3998</v>
+        <v>174.4722</v>
       </c>
       <c r="AO30" s="0">
-        <v>275.9091</v>
+        <v>292.571</v>
       </c>
       <c r="AP30" s="0">
-        <v>239.3408</v>
+        <v>244.3111</v>
       </c>
       <c r="AQ30" s="0">
-        <v>114.6746</v>
+        <v>117.3912</v>
       </c>
       <c r="AR30" s="0">
-        <v>106.2017</v>
+        <v>109.3469</v>
       </c>
       <c r="AS30" s="0">
-        <v>715.4025</v>
+        <v>739.2591</v>
       </c>
       <c r="AT30" s="0">
-        <v>700.0611</v>
+        <v>743.8789</v>
       </c>
       <c r="AU30" s="0">
-        <v>380.783</v>
+        <v>401.603</v>
       </c>
       <c r="AV30" s="0">
-        <v>1301.833</v>
+        <v>1171.342</v>
       </c>
       <c r="AW30" s="0">
-        <v>215.7606</v>
+        <v>222.018</v>
       </c>
       <c r="AX30" s="0">
-        <v>672.6618</v>
+        <v>681.5104</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>2018</v>
+      </c>
+      <c r="B31" s="0">
+        <v>315.1821</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="0">
+        <v>105.4536</v>
+      </c>
+      <c r="E31" s="0">
+        <v>155.3604</v>
+      </c>
+      <c r="F31" s="0">
+        <v>1165.507</v>
+      </c>
+      <c r="G31" s="0">
+        <v>347.4642</v>
+      </c>
+      <c r="H31" s="0">
+        <v>473.4456</v>
+      </c>
+      <c r="I31" s="0">
+        <v>267.6318</v>
+      </c>
+      <c r="J31" s="0">
+        <v>590.2204</v>
+      </c>
+      <c r="K31" s="0">
+        <v>787.3791</v>
+      </c>
+      <c r="L31" s="0">
+        <v>443.1612</v>
+      </c>
+      <c r="M31" s="0">
+        <v>1116.23</v>
+      </c>
+      <c r="N31" s="0">
+        <v>334.2624</v>
+      </c>
+      <c r="O31" s="0">
+        <v>230.8142</v>
+      </c>
+      <c r="P31" s="0">
+        <v>237.8672</v>
+      </c>
+      <c r="Q31" s="0">
+        <v>272.8673</v>
+      </c>
+      <c r="R31" s="0">
+        <v>169.2627</v>
+      </c>
+      <c r="S31" s="0">
+        <v>324.5073</v>
+      </c>
+      <c r="T31" s="0">
+        <v>331.0268</v>
+      </c>
+      <c r="U31" s="0">
+        <v>346.003</v>
+      </c>
+      <c r="V31" s="0">
+        <v>271.6019</v>
+      </c>
+      <c r="W31" s="0">
+        <v>114.6758</v>
+      </c>
+      <c r="X31" s="0">
+        <v>213.7188</v>
+      </c>
+      <c r="Y31" s="0">
+        <v>697.2249</v>
+      </c>
+      <c r="Z31" s="0">
+        <v>502.3463</v>
+      </c>
+      <c r="AA31" s="0">
+        <v>240.15</v>
+      </c>
+      <c r="AB31" s="0">
+        <v>179.3139</v>
+      </c>
+      <c r="AC31" s="0">
+        <v>129.7346</v>
+      </c>
+      <c r="AD31" s="0">
+        <v>679.9527</v>
+      </c>
+      <c r="AE31" s="0">
+        <v>531.8051</v>
+      </c>
+      <c r="AF31" s="0">
+        <v>400.9866</v>
+      </c>
+      <c r="AG31" s="0">
+        <v>169.1111</v>
+      </c>
+      <c r="AH31" s="0">
+        <v>321.5958</v>
+      </c>
+      <c r="AI31" s="0">
+        <v>1373.722</v>
+      </c>
+      <c r="AJ31" s="0">
+        <v>1294.071</v>
+      </c>
+      <c r="AK31" s="0">
+        <v>841.5776</v>
+      </c>
+      <c r="AL31" s="0">
+        <v>628.7115</v>
+      </c>
+      <c r="AM31" s="0">
+        <v>1116.09</v>
+      </c>
+      <c r="AN31" s="0">
+        <v>177.8114</v>
+      </c>
+      <c r="AO31" s="0">
+        <v>326.8972</v>
+      </c>
+      <c r="AP31" s="0">
+        <v>247.5243</v>
+      </c>
+      <c r="AQ31" s="0">
+        <v>122.3093</v>
+      </c>
+      <c r="AR31" s="0">
+        <v>110.8435</v>
+      </c>
+      <c r="AS31" s="0">
+        <v>732.5507</v>
+      </c>
+      <c r="AT31" s="0">
+        <v>804.7305</v>
+      </c>
+      <c r="AU31" s="0">
+        <v>412.415</v>
+      </c>
+      <c r="AV31" s="0">
+        <v>836.5415</v>
+      </c>
+      <c r="AW31" s="0">
+        <v>225.5924</v>
+      </c>
+      <c r="AX31" s="0">
+        <v>696.3544</v>
       </c>
     </row>
   </sheetData>
@@ -5770,7 +5961,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AX331"/>
+  <dimension ref="A1:AX344"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -55941,7 +56132,7 @@
         <v>379</v>
       </c>
       <c r="B331" s="0">
-        <v>310.1862</v>
+        <v>310.3837</v>
       </c>
       <c r="C331" s="0" t="s">
         <v>50</v>
@@ -55950,142 +56141,2118 @@
         <v>50</v>
       </c>
       <c r="E331" s="0">
-        <v>156.7992</v>
+        <v>155.8646</v>
       </c>
       <c r="F331" s="0">
-        <v>1132.338</v>
+        <v>1131.676</v>
       </c>
       <c r="G331" s="0">
-        <v>343.1394</v>
+        <v>343.5542</v>
       </c>
       <c r="H331" s="0">
-        <v>471.5216</v>
+        <v>471.8525</v>
       </c>
       <c r="I331" s="0">
-        <v>253.1732</v>
+        <v>253.3455</v>
       </c>
       <c r="J331" s="0">
-        <v>577.11</v>
+        <v>577.4392</v>
       </c>
       <c r="K331" s="0">
-        <v>781.5562</v>
+        <v>782.2889</v>
       </c>
       <c r="L331" s="0">
-        <v>425.8223</v>
+        <v>426.1649</v>
       </c>
       <c r="M331" s="0">
-        <v>1016.976</v>
+        <v>1017.225</v>
       </c>
       <c r="N331" s="0">
-        <v>315.6637</v>
+        <v>315.6239</v>
       </c>
       <c r="O331" s="0">
-        <v>219.5178</v>
+        <v>219.8637</v>
       </c>
       <c r="P331" s="0">
-        <v>229.3731</v>
+        <v>229.5309</v>
       </c>
       <c r="Q331" s="0">
-        <v>237.2408</v>
+        <v>238.0465</v>
       </c>
       <c r="R331" s="0">
-        <v>164.4323</v>
+        <v>164.5896</v>
       </c>
       <c r="S331" s="0">
-        <v>320.3796</v>
+        <v>320.5753</v>
       </c>
       <c r="T331" s="0">
-        <v>326.1968</v>
+        <v>326.5907</v>
       </c>
       <c r="U331" s="0">
-        <v>309.6959</v>
+        <v>310.6251</v>
       </c>
       <c r="V331" s="0">
-        <v>257.2084</v>
+        <v>257.6955</v>
       </c>
       <c r="W331" s="0">
-        <v>112.0204</v>
+        <v>112.1303</v>
       </c>
       <c r="X331" s="0">
-        <v>204.3424</v>
+        <v>204.5221</v>
       </c>
       <c r="Y331" s="0">
-        <v>699.5479</v>
+        <v>700.2286</v>
       </c>
       <c r="Z331" s="0">
-        <v>513.6075</v>
+        <v>513.4411</v>
       </c>
       <c r="AA331" s="0">
-        <v>235.6486</v>
+        <v>235.776</v>
       </c>
       <c r="AB331" s="0">
-        <v>178.2993</v>
+        <v>178.3555</v>
       </c>
       <c r="AC331" s="0">
-        <v>127.9149</v>
+        <v>128.0544</v>
       </c>
       <c r="AD331" s="0">
-        <v>670.4325</v>
+        <v>671.0194</v>
       </c>
       <c r="AE331" s="0">
-        <v>535.6836</v>
+        <v>535.8772</v>
       </c>
       <c r="AF331" s="0">
-        <v>394.256</v>
+        <v>394.6023</v>
       </c>
       <c r="AG331" s="0">
-        <v>161.3862</v>
+        <v>161.6575</v>
       </c>
       <c r="AH331" s="0">
-        <v>318.6147</v>
+        <v>318.7653</v>
       </c>
       <c r="AI331" s="0">
-        <v>1342.772</v>
+        <v>1343.885</v>
       </c>
       <c r="AJ331" s="0">
-        <v>1274.782</v>
+        <v>1276.46</v>
       </c>
       <c r="AK331" s="0">
-        <v>846.4003</v>
+        <v>846.7976</v>
       </c>
       <c r="AL331" s="0">
-        <v>624.4434</v>
+        <v>625.0639</v>
       </c>
       <c r="AM331" s="0">
-        <v>1114.632</v>
+        <v>1115.307</v>
       </c>
       <c r="AN331" s="0">
-        <v>173.0445</v>
+        <v>173.351</v>
       </c>
       <c r="AO331" s="0">
-        <v>278.8592</v>
+        <v>279.2232</v>
       </c>
       <c r="AP331" s="0">
-        <v>242.8337</v>
+        <v>242.9449</v>
       </c>
       <c r="AQ331" s="0">
-        <v>115.2755</v>
+        <v>115.3255</v>
       </c>
       <c r="AR331" s="0">
-        <v>109.265</v>
+        <v>109.1092</v>
       </c>
       <c r="AS331" s="0">
-        <v>742.0132</v>
+        <v>743.1958</v>
       </c>
       <c r="AT331" s="0">
-        <v>726.1553</v>
+        <v>727.2636</v>
       </c>
       <c r="AU331" s="0">
-        <v>390.9775</v>
+        <v>391.4898</v>
       </c>
       <c r="AV331" s="0">
-        <v>1308.952</v>
+        <v>1314.352</v>
       </c>
       <c r="AW331" s="0">
-        <v>219.3083</v>
+        <v>219.5223</v>
       </c>
       <c r="AX331" s="0">
-        <v>679.8239</v>
+        <v>680.6609</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B332" s="0">
+        <v>313.2231</v>
+      </c>
+      <c r="C332" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D332" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E332" s="0">
+        <v>150.3216</v>
+      </c>
+      <c r="F332" s="0">
+        <v>1131.757</v>
+      </c>
+      <c r="G332" s="0">
+        <v>348.7304</v>
+      </c>
+      <c r="H332" s="0">
+        <v>475.789</v>
+      </c>
+      <c r="I332" s="0">
+        <v>256.5779</v>
+      </c>
+      <c r="J332" s="0">
+        <v>585.9471</v>
+      </c>
+      <c r="K332" s="0">
+        <v>789.0706</v>
+      </c>
+      <c r="L332" s="0">
+        <v>432.8783</v>
+      </c>
+      <c r="M332" s="0">
+        <v>1009.299</v>
+      </c>
+      <c r="N332" s="0">
+        <v>315.2223</v>
+      </c>
+      <c r="O332" s="0">
+        <v>220.0537</v>
+      </c>
+      <c r="P332" s="0">
+        <v>231.3503</v>
+      </c>
+      <c r="Q332" s="0">
+        <v>245.027</v>
+      </c>
+      <c r="R332" s="0">
+        <v>167.1934</v>
+      </c>
+      <c r="S332" s="0">
+        <v>324.4161</v>
+      </c>
+      <c r="T332" s="0">
+        <v>331.271</v>
+      </c>
+      <c r="U332" s="0">
+        <v>312.4435</v>
+      </c>
+      <c r="V332" s="0">
+        <v>261.6836</v>
+      </c>
+      <c r="W332" s="0">
+        <v>113.3755</v>
+      </c>
+      <c r="X332" s="0">
+        <v>206.2913</v>
+      </c>
+      <c r="Y332" s="0">
+        <v>705.4266</v>
+      </c>
+      <c r="Z332" s="0">
+        <v>514.0635</v>
+      </c>
+      <c r="AA332" s="0">
+        <v>237.6132</v>
+      </c>
+      <c r="AB332" s="0">
+        <v>179.7725</v>
+      </c>
+      <c r="AC332" s="0">
+        <v>129.8512</v>
+      </c>
+      <c r="AD332" s="0">
+        <v>679.6829</v>
+      </c>
+      <c r="AE332" s="0">
+        <v>535.6541</v>
+      </c>
+      <c r="AF332" s="0">
+        <v>399.8843</v>
+      </c>
+      <c r="AG332" s="0">
+        <v>162.2367</v>
+      </c>
+      <c r="AH332" s="0">
+        <v>323.1272</v>
+      </c>
+      <c r="AI332" s="0">
+        <v>1361.812</v>
+      </c>
+      <c r="AJ332" s="0">
+        <v>1296.477</v>
+      </c>
+      <c r="AK332" s="0">
+        <v>859.2395</v>
+      </c>
+      <c r="AL332" s="0">
+        <v>634.8366</v>
+      </c>
+      <c r="AM332" s="0">
+        <v>1117.385</v>
+      </c>
+      <c r="AN332" s="0">
+        <v>174.9762</v>
+      </c>
+      <c r="AO332" s="0">
+        <v>285.3675</v>
+      </c>
+      <c r="AP332" s="0">
+        <v>245.4975</v>
+      </c>
+      <c r="AQ332" s="0">
+        <v>115.6137</v>
+      </c>
+      <c r="AR332" s="0">
+        <v>108.6509</v>
+      </c>
+      <c r="AS332" s="0">
+        <v>753.0497</v>
+      </c>
+      <c r="AT332" s="0">
+        <v>737.5254</v>
+      </c>
+      <c r="AU332" s="0">
+        <v>403.1338</v>
+      </c>
+      <c r="AV332" s="0">
+        <v>1266.312</v>
+      </c>
+      <c r="AW332" s="0">
+        <v>222.4599</v>
+      </c>
+      <c r="AX332" s="0">
+        <v>684.5675</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="B333" s="0">
+        <v>307.0583</v>
+      </c>
+      <c r="C333" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D333" s="0">
+        <v>100</v>
+      </c>
+      <c r="E333" s="0">
+        <v>151.72</v>
+      </c>
+      <c r="F333" s="0">
+        <v>1138.9</v>
+      </c>
+      <c r="G333" s="0">
+        <v>347.9345</v>
+      </c>
+      <c r="H333" s="0">
+        <v>475.3736</v>
+      </c>
+      <c r="I333" s="0">
+        <v>256.6299</v>
+      </c>
+      <c r="J333" s="0">
+        <v>580.3979</v>
+      </c>
+      <c r="K333" s="0">
+        <v>786.2865</v>
+      </c>
+      <c r="L333" s="0">
+        <v>433.8236</v>
+      </c>
+      <c r="M333" s="0">
+        <v>1025.562</v>
+      </c>
+      <c r="N333" s="0">
+        <v>317.5771</v>
+      </c>
+      <c r="O333" s="0">
+        <v>215.4965</v>
+      </c>
+      <c r="P333" s="0">
+        <v>231.4337</v>
+      </c>
+      <c r="Q333" s="0">
+        <v>245.3899</v>
+      </c>
+      <c r="R333" s="0">
+        <v>167.4078</v>
+      </c>
+      <c r="S333" s="0">
+        <v>324.0184</v>
+      </c>
+      <c r="T333" s="0">
+        <v>330.8118</v>
+      </c>
+      <c r="U333" s="0">
+        <v>310.6144</v>
+      </c>
+      <c r="V333" s="0">
+        <v>262.0889</v>
+      </c>
+      <c r="W333" s="0">
+        <v>112.58</v>
+      </c>
+      <c r="X333" s="0">
+        <v>204.3799</v>
+      </c>
+      <c r="Y333" s="0">
+        <v>702.0415</v>
+      </c>
+      <c r="Z333" s="0">
+        <v>509.1174</v>
+      </c>
+      <c r="AA333" s="0">
+        <v>237.8685</v>
+      </c>
+      <c r="AB333" s="0">
+        <v>179.3239</v>
+      </c>
+      <c r="AC333" s="0">
+        <v>129.5332</v>
+      </c>
+      <c r="AD333" s="0">
+        <v>678.7455</v>
+      </c>
+      <c r="AE333" s="0">
+        <v>532.0757</v>
+      </c>
+      <c r="AF333" s="0">
+        <v>399.7633</v>
+      </c>
+      <c r="AG333" s="0">
+        <v>162.3641</v>
+      </c>
+      <c r="AH333" s="0">
+        <v>321.1906</v>
+      </c>
+      <c r="AI333" s="0">
+        <v>1360.771</v>
+      </c>
+      <c r="AJ333" s="0">
+        <v>1289.852</v>
+      </c>
+      <c r="AK333" s="0">
+        <v>856.9716</v>
+      </c>
+      <c r="AL333" s="0">
+        <v>631.0704</v>
+      </c>
+      <c r="AM333" s="0">
+        <v>1114.722</v>
+      </c>
+      <c r="AN333" s="0">
+        <v>175.0419</v>
+      </c>
+      <c r="AO333" s="0">
+        <v>286.1093</v>
+      </c>
+      <c r="AP333" s="0">
+        <v>245.7099</v>
+      </c>
+      <c r="AQ333" s="0">
+        <v>116.8208</v>
+      </c>
+      <c r="AR333" s="0">
+        <v>107.9678</v>
+      </c>
+      <c r="AS333" s="0">
+        <v>748.5402</v>
+      </c>
+      <c r="AT333" s="0">
+        <v>746.0607</v>
+      </c>
+      <c r="AU333" s="0">
+        <v>404.2867</v>
+      </c>
+      <c r="AV333" s="0">
+        <v>1224.792</v>
+      </c>
+      <c r="AW333" s="0">
+        <v>223.1732</v>
+      </c>
+      <c r="AX333" s="0">
+        <v>677.3122</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B334" s="0">
+        <v>314.6261</v>
+      </c>
+      <c r="C334" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D334" s="0">
+        <v>101.1343</v>
+      </c>
+      <c r="E334" s="0">
+        <v>153.2755</v>
+      </c>
+      <c r="F334" s="0">
+        <v>1156.226</v>
+      </c>
+      <c r="G334" s="0">
+        <v>352.3483</v>
+      </c>
+      <c r="H334" s="0">
+        <v>479.8611</v>
+      </c>
+      <c r="I334" s="0">
+        <v>263.3813</v>
+      </c>
+      <c r="J334" s="0">
+        <v>587.5414</v>
+      </c>
+      <c r="K334" s="0">
+        <v>795.7098</v>
+      </c>
+      <c r="L334" s="0">
+        <v>444.1007</v>
+      </c>
+      <c r="M334" s="0">
+        <v>1059.226</v>
+      </c>
+      <c r="N334" s="0">
+        <v>324.7193</v>
+      </c>
+      <c r="O334" s="0">
+        <v>221.8748</v>
+      </c>
+      <c r="P334" s="0">
+        <v>233.5368</v>
+      </c>
+      <c r="Q334" s="0">
+        <v>253.2651</v>
+      </c>
+      <c r="R334" s="0">
+        <v>169.2409</v>
+      </c>
+      <c r="S334" s="0">
+        <v>327.9945</v>
+      </c>
+      <c r="T334" s="0">
+        <v>335.6142</v>
+      </c>
+      <c r="U334" s="0">
+        <v>328.4086</v>
+      </c>
+      <c r="V334" s="0">
+        <v>266.4472</v>
+      </c>
+      <c r="W334" s="0">
+        <v>114.2727</v>
+      </c>
+      <c r="X334" s="0">
+        <v>209.1574</v>
+      </c>
+      <c r="Y334" s="0">
+        <v>708.2351</v>
+      </c>
+      <c r="Z334" s="0">
+        <v>511.7914</v>
+      </c>
+      <c r="AA334" s="0">
+        <v>243.4078</v>
+      </c>
+      <c r="AB334" s="0">
+        <v>180.1339</v>
+      </c>
+      <c r="AC334" s="0">
+        <v>131.9034</v>
+      </c>
+      <c r="AD334" s="0">
+        <v>690.1185</v>
+      </c>
+      <c r="AE334" s="0">
+        <v>537.99</v>
+      </c>
+      <c r="AF334" s="0">
+        <v>402.4234</v>
+      </c>
+      <c r="AG334" s="0">
+        <v>165.9736</v>
+      </c>
+      <c r="AH334" s="0">
+        <v>323.8704</v>
+      </c>
+      <c r="AI334" s="0">
+        <v>1379.818</v>
+      </c>
+      <c r="AJ334" s="0">
+        <v>1310.601</v>
+      </c>
+      <c r="AK334" s="0">
+        <v>864.8444</v>
+      </c>
+      <c r="AL334" s="0">
+        <v>637.0279</v>
+      </c>
+      <c r="AM334" s="0">
+        <v>1125.392</v>
+      </c>
+      <c r="AN334" s="0">
+        <v>177.9641</v>
+      </c>
+      <c r="AO334" s="0">
+        <v>291.8276</v>
+      </c>
+      <c r="AP334" s="0">
+        <v>248.0173</v>
+      </c>
+      <c r="AQ334" s="0">
+        <v>119.0266</v>
+      </c>
+      <c r="AR334" s="0">
+        <v>110.7102</v>
+      </c>
+      <c r="AS334" s="0">
+        <v>764.4388</v>
+      </c>
+      <c r="AT334" s="0">
+        <v>760.1128</v>
+      </c>
+      <c r="AU334" s="0">
+        <v>411.2404</v>
+      </c>
+      <c r="AV334" s="0">
+        <v>1112.674</v>
+      </c>
+      <c r="AW334" s="0">
+        <v>225.1702</v>
+      </c>
+      <c r="AX334" s="0">
+        <v>688.8903</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="B335" s="0">
+        <v>325.7467</v>
+      </c>
+      <c r="C335" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D335" s="0">
+        <v>103.2158</v>
+      </c>
+      <c r="E335" s="0">
+        <v>158.7616</v>
+      </c>
+      <c r="F335" s="0">
+        <v>1173.075</v>
+      </c>
+      <c r="G335" s="0">
+        <v>354.9358</v>
+      </c>
+      <c r="H335" s="0">
+        <v>482.1215</v>
+      </c>
+      <c r="I335" s="0">
+        <v>266.7595</v>
+      </c>
+      <c r="J335" s="0">
+        <v>596.2766</v>
+      </c>
+      <c r="K335" s="0">
+        <v>805.346</v>
+      </c>
+      <c r="L335" s="0">
+        <v>450.3855</v>
+      </c>
+      <c r="M335" s="0">
+        <v>1072.936</v>
+      </c>
+      <c r="N335" s="0">
+        <v>330.598</v>
+      </c>
+      <c r="O335" s="0">
+        <v>222.2829</v>
+      </c>
+      <c r="P335" s="0">
+        <v>237.2542</v>
+      </c>
+      <c r="Q335" s="0">
+        <v>258.1385</v>
+      </c>
+      <c r="R335" s="0">
+        <v>170.5593</v>
+      </c>
+      <c r="S335" s="0">
+        <v>331.2728</v>
+      </c>
+      <c r="T335" s="0">
+        <v>340.4071</v>
+      </c>
+      <c r="U335" s="0">
+        <v>328.9319</v>
+      </c>
+      <c r="V335" s="0">
+        <v>274.0704</v>
+      </c>
+      <c r="W335" s="0">
+        <v>114.6055</v>
+      </c>
+      <c r="X335" s="0">
+        <v>213.0669</v>
+      </c>
+      <c r="Y335" s="0">
+        <v>719.647</v>
+      </c>
+      <c r="Z335" s="0">
+        <v>514.7705</v>
+      </c>
+      <c r="AA335" s="0">
+        <v>246.6709</v>
+      </c>
+      <c r="AB335" s="0">
+        <v>181.0646</v>
+      </c>
+      <c r="AC335" s="0">
+        <v>133.1739</v>
+      </c>
+      <c r="AD335" s="0">
+        <v>698.9501</v>
+      </c>
+      <c r="AE335" s="0">
+        <v>540.771</v>
+      </c>
+      <c r="AF335" s="0">
+        <v>404.9827</v>
+      </c>
+      <c r="AG335" s="0">
+        <v>168.3679</v>
+      </c>
+      <c r="AH335" s="0">
+        <v>326.3869</v>
+      </c>
+      <c r="AI335" s="0">
+        <v>1403.79</v>
+      </c>
+      <c r="AJ335" s="0">
+        <v>1332.18</v>
+      </c>
+      <c r="AK335" s="0">
+        <v>871.1891</v>
+      </c>
+      <c r="AL335" s="0">
+        <v>640.2761</v>
+      </c>
+      <c r="AM335" s="0">
+        <v>1133.469</v>
+      </c>
+      <c r="AN335" s="0">
+        <v>180.2594</v>
+      </c>
+      <c r="AO335" s="0">
+        <v>304.5514</v>
+      </c>
+      <c r="AP335" s="0">
+        <v>248.737</v>
+      </c>
+      <c r="AQ335" s="0">
+        <v>120.145</v>
+      </c>
+      <c r="AR335" s="0">
+        <v>112.3723</v>
+      </c>
+      <c r="AS335" s="0">
+        <v>767.0001</v>
+      </c>
+      <c r="AT335" s="0">
+        <v>788.1268</v>
+      </c>
+      <c r="AU335" s="0">
+        <v>419.3093</v>
+      </c>
+      <c r="AV335" s="0">
+        <v>1115.689</v>
+      </c>
+      <c r="AW335" s="0">
+        <v>227.4769</v>
+      </c>
+      <c r="AX335" s="0">
+        <v>695.1902</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="B336" s="0">
+        <v>330.2703</v>
+      </c>
+      <c r="C336" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D336" s="0">
+        <v>103.7922</v>
+      </c>
+      <c r="E336" s="0">
+        <v>161.9452</v>
+      </c>
+      <c r="F336" s="0">
+        <v>1180.037</v>
+      </c>
+      <c r="G336" s="0">
+        <v>354.3815</v>
+      </c>
+      <c r="H336" s="0">
+        <v>481.942</v>
+      </c>
+      <c r="I336" s="0">
+        <v>267.4821</v>
+      </c>
+      <c r="J336" s="0">
+        <v>593.8723</v>
+      </c>
+      <c r="K336" s="0">
+        <v>804.6338</v>
+      </c>
+      <c r="L336" s="0">
+        <v>449.8513</v>
+      </c>
+      <c r="M336" s="0">
+        <v>1100.152</v>
+      </c>
+      <c r="N336" s="0">
+        <v>330.9285</v>
+      </c>
+      <c r="O336" s="0">
+        <v>224.1007</v>
+      </c>
+      <c r="P336" s="0">
+        <v>238.2426</v>
+      </c>
+      <c r="Q336" s="0">
+        <v>262.7612</v>
+      </c>
+      <c r="R336" s="0">
+        <v>170.2461</v>
+      </c>
+      <c r="S336" s="0">
+        <v>330.3672</v>
+      </c>
+      <c r="T336" s="0">
+        <v>340.4912</v>
+      </c>
+      <c r="U336" s="0">
+        <v>327.8767</v>
+      </c>
+      <c r="V336" s="0">
+        <v>275.6981</v>
+      </c>
+      <c r="W336" s="0">
+        <v>114.655</v>
+      </c>
+      <c r="X336" s="0">
+        <v>213.0492</v>
+      </c>
+      <c r="Y336" s="0">
+        <v>720.2223</v>
+      </c>
+      <c r="Z336" s="0">
+        <v>513.2567</v>
+      </c>
+      <c r="AA336" s="0">
+        <v>247.607</v>
+      </c>
+      <c r="AB336" s="0">
+        <v>181.2542</v>
+      </c>
+      <c r="AC336" s="0">
+        <v>131.6352</v>
+      </c>
+      <c r="AD336" s="0">
+        <v>692.3655</v>
+      </c>
+      <c r="AE336" s="0">
+        <v>539.2168</v>
+      </c>
+      <c r="AF336" s="0">
+        <v>406.0664</v>
+      </c>
+      <c r="AG336" s="0">
+        <v>166.8564</v>
+      </c>
+      <c r="AH336" s="0">
+        <v>326.3551</v>
+      </c>
+      <c r="AI336" s="0">
+        <v>1397.816</v>
+      </c>
+      <c r="AJ336" s="0">
+        <v>1324.361</v>
+      </c>
+      <c r="AK336" s="0">
+        <v>865.6678</v>
+      </c>
+      <c r="AL336" s="0">
+        <v>638.4602</v>
+      </c>
+      <c r="AM336" s="0">
+        <v>1129.901</v>
+      </c>
+      <c r="AN336" s="0">
+        <v>181.4841</v>
+      </c>
+      <c r="AO336" s="0">
+        <v>316.2143</v>
+      </c>
+      <c r="AP336" s="0">
+        <v>248.5766</v>
+      </c>
+      <c r="AQ336" s="0">
+        <v>120.2755</v>
+      </c>
+      <c r="AR336" s="0">
+        <v>112.3319</v>
+      </c>
+      <c r="AS336" s="0">
+        <v>757.8747</v>
+      </c>
+      <c r="AT336" s="0">
+        <v>793.3496</v>
+      </c>
+      <c r="AU336" s="0">
+        <v>419.7182</v>
+      </c>
+      <c r="AV336" s="0">
+        <v>1125.92</v>
+      </c>
+      <c r="AW336" s="0">
+        <v>228.7779</v>
+      </c>
+      <c r="AX336" s="0">
+        <v>689.7772</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="B337" s="0">
+        <v>330.1189</v>
+      </c>
+      <c r="C337" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D337" s="0">
+        <v>102.645</v>
+      </c>
+      <c r="E337" s="0">
+        <v>155.1837</v>
+      </c>
+      <c r="F337" s="0">
+        <v>1181.904</v>
+      </c>
+      <c r="G337" s="0">
+        <v>355.4273</v>
+      </c>
+      <c r="H337" s="0">
+        <v>482.1311</v>
+      </c>
+      <c r="I337" s="0">
+        <v>269.063</v>
+      </c>
+      <c r="J337" s="0">
+        <v>596.8145</v>
+      </c>
+      <c r="K337" s="0">
+        <v>800.4916</v>
+      </c>
+      <c r="L337" s="0">
+        <v>450.8549</v>
+      </c>
+      <c r="M337" s="0">
+        <v>1123.759</v>
+      </c>
+      <c r="N337" s="0">
+        <v>334.8871</v>
+      </c>
+      <c r="O337" s="0">
+        <v>226.6121</v>
+      </c>
+      <c r="P337" s="0">
+        <v>239.6498</v>
+      </c>
+      <c r="Q337" s="0">
+        <v>265.5703</v>
+      </c>
+      <c r="R337" s="0">
+        <v>170.3487</v>
+      </c>
+      <c r="S337" s="0">
+        <v>330.0208</v>
+      </c>
+      <c r="T337" s="0">
+        <v>339.7941</v>
+      </c>
+      <c r="U337" s="0">
+        <v>335.2878</v>
+      </c>
+      <c r="V337" s="0">
+        <v>276.3206</v>
+      </c>
+      <c r="W337" s="0">
+        <v>114.9521</v>
+      </c>
+      <c r="X337" s="0">
+        <v>215.1184</v>
+      </c>
+      <c r="Y337" s="0">
+        <v>713.9695</v>
+      </c>
+      <c r="Z337" s="0">
+        <v>491.5568</v>
+      </c>
+      <c r="AA337" s="0">
+        <v>246.9454</v>
+      </c>
+      <c r="AB337" s="0">
+        <v>181.4357</v>
+      </c>
+      <c r="AC337" s="0">
+        <v>131.4185</v>
+      </c>
+      <c r="AD337" s="0">
+        <v>695.7638</v>
+      </c>
+      <c r="AE337" s="0">
+        <v>527.9686</v>
+      </c>
+      <c r="AF337" s="0">
+        <v>408.6856</v>
+      </c>
+      <c r="AG337" s="0">
+        <v>168.6006</v>
+      </c>
+      <c r="AH337" s="0">
+        <v>323.0053</v>
+      </c>
+      <c r="AI337" s="0">
+        <v>1410.213</v>
+      </c>
+      <c r="AJ337" s="0">
+        <v>1334.391</v>
+      </c>
+      <c r="AK337" s="0">
+        <v>864.2645</v>
+      </c>
+      <c r="AL337" s="0">
+        <v>637.945</v>
+      </c>
+      <c r="AM337" s="0">
+        <v>1132.887</v>
+      </c>
+      <c r="AN337" s="0">
+        <v>182.0162</v>
+      </c>
+      <c r="AO337" s="0">
+        <v>320.0802</v>
+      </c>
+      <c r="AP337" s="0">
+        <v>248.9659</v>
+      </c>
+      <c r="AQ337" s="0">
+        <v>121.0454</v>
+      </c>
+      <c r="AR337" s="0">
+        <v>114.1317</v>
+      </c>
+      <c r="AS337" s="0">
+        <v>743.1739</v>
+      </c>
+      <c r="AT337" s="0">
+        <v>797.6631</v>
+      </c>
+      <c r="AU337" s="0">
+        <v>426.0023</v>
+      </c>
+      <c r="AV337" s="0">
+        <v>881.6807</v>
+      </c>
+      <c r="AW337" s="0">
+        <v>228.8298</v>
+      </c>
+      <c r="AX337" s="0">
+        <v>682.5887</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B338" s="0">
+        <v>334.2042</v>
+      </c>
+      <c r="C338" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D338" s="0">
+        <v>104.2834</v>
+      </c>
+      <c r="E338" s="0">
+        <v>152.9791</v>
+      </c>
+      <c r="F338" s="0">
+        <v>1191.469</v>
+      </c>
+      <c r="G338" s="0">
+        <v>358.4847</v>
+      </c>
+      <c r="H338" s="0">
+        <v>480.7642</v>
+      </c>
+      <c r="I338" s="0">
+        <v>273.3235</v>
+      </c>
+      <c r="J338" s="0">
+        <v>605.1751</v>
+      </c>
+      <c r="K338" s="0">
+        <v>805.6224</v>
+      </c>
+      <c r="L338" s="0">
+        <v>454.0797</v>
+      </c>
+      <c r="M338" s="0">
+        <v>1171.046</v>
+      </c>
+      <c r="N338" s="0">
+        <v>338.042</v>
+      </c>
+      <c r="O338" s="0">
+        <v>233.0704</v>
+      </c>
+      <c r="P338" s="0">
+        <v>241.5289</v>
+      </c>
+      <c r="Q338" s="0">
+        <v>270.6924</v>
+      </c>
+      <c r="R338" s="0">
+        <v>171.0644</v>
+      </c>
+      <c r="S338" s="0">
+        <v>330.9822</v>
+      </c>
+      <c r="T338" s="0">
+        <v>341.1567</v>
+      </c>
+      <c r="U338" s="0">
+        <v>342.3328</v>
+      </c>
+      <c r="V338" s="0">
+        <v>274.6393</v>
+      </c>
+      <c r="W338" s="0">
+        <v>116.6214</v>
+      </c>
+      <c r="X338" s="0">
+        <v>218.4371</v>
+      </c>
+      <c r="Y338" s="0">
+        <v>717.4021</v>
+      </c>
+      <c r="Z338" s="0">
+        <v>502.8719</v>
+      </c>
+      <c r="AA338" s="0">
+        <v>247.5469</v>
+      </c>
+      <c r="AB338" s="0">
+        <v>181.3321</v>
+      </c>
+      <c r="AC338" s="0">
+        <v>133.3699</v>
+      </c>
+      <c r="AD338" s="0">
+        <v>699.5957</v>
+      </c>
+      <c r="AE338" s="0">
+        <v>536.0125</v>
+      </c>
+      <c r="AF338" s="0">
+        <v>408.9845</v>
+      </c>
+      <c r="AG338" s="0">
+        <v>171.6015</v>
+      </c>
+      <c r="AH338" s="0">
+        <v>325.3126</v>
+      </c>
+      <c r="AI338" s="0">
+        <v>1414.664</v>
+      </c>
+      <c r="AJ338" s="0">
+        <v>1340.27</v>
+      </c>
+      <c r="AK338" s="0">
+        <v>866.7303</v>
+      </c>
+      <c r="AL338" s="0">
+        <v>638.6234</v>
+      </c>
+      <c r="AM338" s="0">
+        <v>1137.08</v>
+      </c>
+      <c r="AN338" s="0">
+        <v>184.6191</v>
+      </c>
+      <c r="AO338" s="0">
+        <v>326.7916</v>
+      </c>
+      <c r="AP338" s="0">
+        <v>249.4141</v>
+      </c>
+      <c r="AQ338" s="0">
+        <v>122.3439</v>
+      </c>
+      <c r="AR338" s="0">
+        <v>115.1453</v>
+      </c>
+      <c r="AS338" s="0">
+        <v>758.8371</v>
+      </c>
+      <c r="AT338" s="0">
+        <v>802.295</v>
+      </c>
+      <c r="AU338" s="0">
+        <v>431.118</v>
+      </c>
+      <c r="AV338" s="0">
+        <v>814.4782</v>
+      </c>
+      <c r="AW338" s="0">
+        <v>229.3115</v>
+      </c>
+      <c r="AX338" s="0">
+        <v>695.6531</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B339" s="0">
+        <v>330.0022</v>
+      </c>
+      <c r="C339" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D339" s="0">
+        <v>108.0205</v>
+      </c>
+      <c r="E339" s="0">
+        <v>152.4645</v>
+      </c>
+      <c r="F339" s="0">
+        <v>1194.814</v>
+      </c>
+      <c r="G339" s="0">
+        <v>357.1162</v>
+      </c>
+      <c r="H339" s="0">
+        <v>478.6045</v>
+      </c>
+      <c r="I339" s="0">
+        <v>278.2938</v>
+      </c>
+      <c r="J339" s="0">
+        <v>606.9312</v>
+      </c>
+      <c r="K339" s="0">
+        <v>807.852</v>
+      </c>
+      <c r="L339" s="0">
+        <v>458.1646</v>
+      </c>
+      <c r="M339" s="0">
+        <v>1178.353</v>
+      </c>
+      <c r="N339" s="0">
+        <v>342.1025</v>
+      </c>
+      <c r="O339" s="0">
+        <v>237.1826</v>
+      </c>
+      <c r="P339" s="0">
+        <v>241.7074</v>
+      </c>
+      <c r="Q339" s="0">
+        <v>274.8081</v>
+      </c>
+      <c r="R339" s="0">
+        <v>170.8917</v>
+      </c>
+      <c r="S339" s="0">
+        <v>329.3302</v>
+      </c>
+      <c r="T339" s="0">
+        <v>341.2853</v>
+      </c>
+      <c r="U339" s="0">
+        <v>351.3665</v>
+      </c>
+      <c r="V339" s="0">
+        <v>277.7983</v>
+      </c>
+      <c r="W339" s="0">
+        <v>118.5037</v>
+      </c>
+      <c r="X339" s="0">
+        <v>219.4301</v>
+      </c>
+      <c r="Y339" s="0">
+        <v>717.016</v>
+      </c>
+      <c r="Z339" s="0">
+        <v>519.7412</v>
+      </c>
+      <c r="AA339" s="0">
+        <v>248.4503</v>
+      </c>
+      <c r="AB339" s="0">
+        <v>180.4499</v>
+      </c>
+      <c r="AC339" s="0">
+        <v>134.1254</v>
+      </c>
+      <c r="AD339" s="0">
+        <v>697.7149</v>
+      </c>
+      <c r="AE339" s="0">
+        <v>546.7361</v>
+      </c>
+      <c r="AF339" s="0">
+        <v>407.7191</v>
+      </c>
+      <c r="AG339" s="0">
+        <v>174.3057</v>
+      </c>
+      <c r="AH339" s="0">
+        <v>330.219</v>
+      </c>
+      <c r="AI339" s="0">
+        <v>1418.718</v>
+      </c>
+      <c r="AJ339" s="0">
+        <v>1343.702</v>
+      </c>
+      <c r="AK339" s="0">
+        <v>866.7436</v>
+      </c>
+      <c r="AL339" s="0">
+        <v>634.0592</v>
+      </c>
+      <c r="AM339" s="0">
+        <v>1141.839</v>
+      </c>
+      <c r="AN339" s="0">
+        <v>186.7354</v>
+      </c>
+      <c r="AO339" s="0">
+        <v>334.1509</v>
+      </c>
+      <c r="AP339" s="0">
+        <v>249.5121</v>
+      </c>
+      <c r="AQ339" s="0">
+        <v>123.2064</v>
+      </c>
+      <c r="AR339" s="0">
+        <v>115.2899</v>
+      </c>
+      <c r="AS339" s="0">
+        <v>763.6548</v>
+      </c>
+      <c r="AT339" s="0">
+        <v>825.4533</v>
+      </c>
+      <c r="AU339" s="0">
+        <v>430.867</v>
+      </c>
+      <c r="AV339" s="0">
+        <v>804.7897</v>
+      </c>
+      <c r="AW339" s="0">
+        <v>229.7256</v>
+      </c>
+      <c r="AX339" s="0">
+        <v>708.8023</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="B340" s="0">
+        <v>317.1556</v>
+      </c>
+      <c r="C340" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D340" s="0">
+        <v>106.474</v>
+      </c>
+      <c r="E340" s="0">
+        <v>154.2856</v>
+      </c>
+      <c r="F340" s="0">
+        <v>1172.139</v>
+      </c>
+      <c r="G340" s="0">
+        <v>347.5609</v>
+      </c>
+      <c r="H340" s="0">
+        <v>473.7214</v>
+      </c>
+      <c r="I340" s="0">
+        <v>269.404</v>
+      </c>
+      <c r="J340" s="0">
+        <v>587.5497</v>
+      </c>
+      <c r="K340" s="0">
+        <v>791.6908</v>
+      </c>
+      <c r="L340" s="0">
+        <v>444.5601</v>
+      </c>
+      <c r="M340" s="0">
+        <v>1147.91</v>
+      </c>
+      <c r="N340" s="0">
+        <v>336.7523</v>
+      </c>
+      <c r="O340" s="0">
+        <v>231.3399</v>
+      </c>
+      <c r="P340" s="0">
+        <v>239.8561</v>
+      </c>
+      <c r="Q340" s="0">
+        <v>270.8528</v>
+      </c>
+      <c r="R340" s="0">
+        <v>169.3017</v>
+      </c>
+      <c r="S340" s="0">
+        <v>325.2468</v>
+      </c>
+      <c r="T340" s="0">
+        <v>333.0557</v>
+      </c>
+      <c r="U340" s="0">
+        <v>347.9297</v>
+      </c>
+      <c r="V340" s="0">
+        <v>272.9417</v>
+      </c>
+      <c r="W340" s="0">
+        <v>117.4054</v>
+      </c>
+      <c r="X340" s="0">
+        <v>214.4867</v>
+      </c>
+      <c r="Y340" s="0">
+        <v>699.3534</v>
+      </c>
+      <c r="Z340" s="0">
+        <v>510.3635</v>
+      </c>
+      <c r="AA340" s="0">
+        <v>242.5398</v>
+      </c>
+      <c r="AB340" s="0">
+        <v>179.0883</v>
+      </c>
+      <c r="AC340" s="0">
+        <v>130.4928</v>
+      </c>
+      <c r="AD340" s="0">
+        <v>684.047</v>
+      </c>
+      <c r="AE340" s="0">
+        <v>538.8293</v>
+      </c>
+      <c r="AF340" s="0">
+        <v>402.488</v>
+      </c>
+      <c r="AG340" s="0">
+        <v>168.9326</v>
+      </c>
+      <c r="AH340" s="0">
+        <v>323.4154</v>
+      </c>
+      <c r="AI340" s="0">
+        <v>1380.209</v>
+      </c>
+      <c r="AJ340" s="0">
+        <v>1299.113</v>
+      </c>
+      <c r="AK340" s="0">
+        <v>840.8714</v>
+      </c>
+      <c r="AL340" s="0">
+        <v>628.1866</v>
+      </c>
+      <c r="AM340" s="0">
+        <v>1132.558</v>
+      </c>
+      <c r="AN340" s="0">
+        <v>180.9452</v>
+      </c>
+      <c r="AO340" s="0">
+        <v>326.2636</v>
+      </c>
+      <c r="AP340" s="0">
+        <v>247.238</v>
+      </c>
+      <c r="AQ340" s="0">
+        <v>122.4609</v>
+      </c>
+      <c r="AR340" s="0">
+        <v>112.1588</v>
+      </c>
+      <c r="AS340" s="0">
+        <v>747.5975</v>
+      </c>
+      <c r="AT340" s="0">
+        <v>812.7184</v>
+      </c>
+      <c r="AU340" s="0">
+        <v>415.3195</v>
+      </c>
+      <c r="AV340" s="0">
+        <v>799.0353</v>
+      </c>
+      <c r="AW340" s="0">
+        <v>225.0562</v>
+      </c>
+      <c r="AX340" s="0">
+        <v>699.3776</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B341" s="0">
+        <v>316.5096</v>
+      </c>
+      <c r="C341" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D341" s="0">
+        <v>105.6162</v>
+      </c>
+      <c r="E341" s="0">
+        <v>155.4768</v>
+      </c>
+      <c r="F341" s="0">
+        <v>1172.893</v>
+      </c>
+      <c r="G341" s="0">
+        <v>347.1196</v>
+      </c>
+      <c r="H341" s="0">
+        <v>473.2432</v>
+      </c>
+      <c r="I341" s="0">
+        <v>265.3924</v>
+      </c>
+      <c r="J341" s="0">
+        <v>588.7982</v>
+      </c>
+      <c r="K341" s="0">
+        <v>789.9759</v>
+      </c>
+      <c r="L341" s="0">
+        <v>444.9677</v>
+      </c>
+      <c r="M341" s="0">
+        <v>1126.741</v>
+      </c>
+      <c r="N341" s="0">
+        <v>335.3012</v>
+      </c>
+      <c r="O341" s="0">
+        <v>228.628</v>
+      </c>
+      <c r="P341" s="0">
+        <v>239.2081</v>
+      </c>
+      <c r="Q341" s="0">
+        <v>271.8354</v>
+      </c>
+      <c r="R341" s="0">
+        <v>169.389</v>
+      </c>
+      <c r="S341" s="0">
+        <v>324.7847</v>
+      </c>
+      <c r="T341" s="0">
+        <v>330.4554</v>
+      </c>
+      <c r="U341" s="0">
+        <v>345.3626</v>
+      </c>
+      <c r="V341" s="0">
+        <v>273.3662</v>
+      </c>
+      <c r="W341" s="0">
+        <v>115.9615</v>
+      </c>
+      <c r="X341" s="0">
+        <v>213.4922</v>
+      </c>
+      <c r="Y341" s="0">
+        <v>700.7486</v>
+      </c>
+      <c r="Z341" s="0">
+        <v>512.9776</v>
+      </c>
+      <c r="AA341" s="0">
+        <v>239.095</v>
+      </c>
+      <c r="AB341" s="0">
+        <v>179.3607</v>
+      </c>
+      <c r="AC341" s="0">
+        <v>129.8022</v>
+      </c>
+      <c r="AD341" s="0">
+        <v>682.6346</v>
+      </c>
+      <c r="AE341" s="0">
+        <v>536.3449</v>
+      </c>
+      <c r="AF341" s="0">
+        <v>402.0001</v>
+      </c>
+      <c r="AG341" s="0">
+        <v>168.24</v>
+      </c>
+      <c r="AH341" s="0">
+        <v>319.2784</v>
+      </c>
+      <c r="AI341" s="0">
+        <v>1371.521</v>
+      </c>
+      <c r="AJ341" s="0">
+        <v>1286.741</v>
+      </c>
+      <c r="AK341" s="0">
+        <v>840.4871</v>
+      </c>
+      <c r="AL341" s="0">
+        <v>629.5453</v>
+      </c>
+      <c r="AM341" s="0">
+        <v>1125.921</v>
+      </c>
+      <c r="AN341" s="0">
+        <v>179.2415</v>
+      </c>
+      <c r="AO341" s="0">
+        <v>330.1658</v>
+      </c>
+      <c r="AP341" s="0">
+        <v>247.479</v>
+      </c>
+      <c r="AQ341" s="0">
+        <v>123.0093</v>
+      </c>
+      <c r="AR341" s="0">
+        <v>109.9876</v>
+      </c>
+      <c r="AS341" s="0">
+        <v>740.7641</v>
+      </c>
+      <c r="AT341" s="0">
+        <v>805.2388</v>
+      </c>
+      <c r="AU341" s="0">
+        <v>413.4615</v>
+      </c>
+      <c r="AV341" s="0">
+        <v>872.418</v>
+      </c>
+      <c r="AW341" s="0">
+        <v>225.0979</v>
+      </c>
+      <c r="AX341" s="0">
+        <v>696.1613</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="B342" s="0">
+        <v>319.2406</v>
+      </c>
+      <c r="C342" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D342" s="0">
+        <v>104.9807</v>
+      </c>
+      <c r="E342" s="0">
+        <v>156.3647</v>
+      </c>
+      <c r="F342" s="0">
+        <v>1176.307</v>
+      </c>
+      <c r="G342" s="0">
+        <v>347.7349</v>
+      </c>
+      <c r="H342" s="0">
+        <v>472.1225</v>
+      </c>
+      <c r="I342" s="0">
+        <v>270.0724</v>
+      </c>
+      <c r="J342" s="0">
+        <v>593.402</v>
+      </c>
+      <c r="K342" s="0">
+        <v>790.662</v>
+      </c>
+      <c r="L342" s="0">
+        <v>445.5193</v>
+      </c>
+      <c r="M342" s="0">
+        <v>1106.356</v>
+      </c>
+      <c r="N342" s="0">
+        <v>336.8332</v>
+      </c>
+      <c r="O342" s="0">
+        <v>233.9688</v>
+      </c>
+      <c r="P342" s="0">
+        <v>237.8577</v>
+      </c>
+      <c r="Q342" s="0">
+        <v>275.4213</v>
+      </c>
+      <c r="R342" s="0">
+        <v>169.9405</v>
+      </c>
+      <c r="S342" s="0">
+        <v>324.6277</v>
+      </c>
+      <c r="T342" s="0">
+        <v>331.4055</v>
+      </c>
+      <c r="U342" s="0">
+        <v>347.6244</v>
+      </c>
+      <c r="V342" s="0">
+        <v>273.8514</v>
+      </c>
+      <c r="W342" s="0">
+        <v>115.1365</v>
+      </c>
+      <c r="X342" s="0">
+        <v>213.2908</v>
+      </c>
+      <c r="Y342" s="0">
+        <v>703.0647</v>
+      </c>
+      <c r="Z342" s="0">
+        <v>512.8454</v>
+      </c>
+      <c r="AA342" s="0">
+        <v>239.9254</v>
+      </c>
+      <c r="AB342" s="0">
+        <v>179.584</v>
+      </c>
+      <c r="AC342" s="0">
+        <v>129.5087</v>
+      </c>
+      <c r="AD342" s="0">
+        <v>685.3136</v>
+      </c>
+      <c r="AE342" s="0">
+        <v>534.6628</v>
+      </c>
+      <c r="AF342" s="0">
+        <v>401.0148</v>
+      </c>
+      <c r="AG342" s="0">
+        <v>171.8413</v>
+      </c>
+      <c r="AH342" s="0">
+        <v>322.5105</v>
+      </c>
+      <c r="AI342" s="0">
+        <v>1367.42</v>
+      </c>
+      <c r="AJ342" s="0">
+        <v>1291.487</v>
+      </c>
+      <c r="AK342" s="0">
+        <v>842.1956</v>
+      </c>
+      <c r="AL342" s="0">
+        <v>629.9837</v>
+      </c>
+      <c r="AM342" s="0">
+        <v>1103.407</v>
+      </c>
+      <c r="AN342" s="0">
+        <v>179.7991</v>
+      </c>
+      <c r="AO342" s="0">
+        <v>328.7961</v>
+      </c>
+      <c r="AP342" s="0">
+        <v>248.0611</v>
+      </c>
+      <c r="AQ342" s="0">
+        <v>123.4</v>
+      </c>
+      <c r="AR342" s="0">
+        <v>111.5067</v>
+      </c>
+      <c r="AS342" s="0">
+        <v>739.2798</v>
+      </c>
+      <c r="AT342" s="0">
+        <v>805.6719</v>
+      </c>
+      <c r="AU342" s="0">
+        <v>410.4734</v>
+      </c>
+      <c r="AV342" s="0">
+        <v>888.7829</v>
+      </c>
+      <c r="AW342" s="0">
+        <v>225.2094</v>
+      </c>
+      <c r="AX342" s="0">
+        <v>698.2428</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B343" s="0">
+        <v>304.3766</v>
+      </c>
+      <c r="C343" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D343" s="0">
+        <v>102.8353</v>
+      </c>
+      <c r="E343" s="0">
+        <v>156.2425</v>
+      </c>
+      <c r="F343" s="0">
+        <v>1151.271</v>
+      </c>
+      <c r="G343" s="0">
+        <v>342.3955</v>
+      </c>
+      <c r="H343" s="0">
+        <v>470.4853</v>
+      </c>
+      <c r="I343" s="0">
+        <v>261.8777</v>
+      </c>
+      <c r="J343" s="0">
+        <v>581.5876</v>
+      </c>
+      <c r="K343" s="0">
+        <v>772.6012</v>
+      </c>
+      <c r="L343" s="0">
+        <v>434.0406</v>
+      </c>
+      <c r="M343" s="0">
+        <v>1057.787</v>
+      </c>
+      <c r="N343" s="0">
+        <v>327.6821</v>
+      </c>
+      <c r="O343" s="0">
+        <v>226.9164</v>
+      </c>
+      <c r="P343" s="0">
+        <v>234.1939</v>
+      </c>
+      <c r="Q343" s="0">
+        <v>273.5428</v>
+      </c>
+      <c r="R343" s="0">
+        <v>168.011</v>
+      </c>
+      <c r="S343" s="0">
+        <v>321.3049</v>
+      </c>
+      <c r="T343" s="0">
+        <v>324.612</v>
+      </c>
+      <c r="U343" s="0">
+        <v>341.2124</v>
+      </c>
+      <c r="V343" s="0">
+        <v>266.0767</v>
+      </c>
+      <c r="W343" s="0">
+        <v>111.0313</v>
+      </c>
+      <c r="X343" s="0">
+        <v>210.1886</v>
+      </c>
+      <c r="Y343" s="0">
+        <v>682.735</v>
+      </c>
+      <c r="Z343" s="0">
+        <v>484.7353</v>
+      </c>
+      <c r="AA343" s="0">
+        <v>235.36</v>
+      </c>
+      <c r="AB343" s="0">
+        <v>178.5374</v>
+      </c>
+      <c r="AC343" s="0">
+        <v>126.9984</v>
+      </c>
+      <c r="AD343" s="0">
+        <v>667.8707</v>
+      </c>
+      <c r="AE343" s="0">
+        <v>518.4341</v>
+      </c>
+      <c r="AF343" s="0">
+        <v>395.7309</v>
+      </c>
+      <c r="AG343" s="0">
+        <v>166.2936</v>
+      </c>
+      <c r="AH343" s="0">
+        <v>317.5273</v>
+      </c>
+      <c r="AI343" s="0">
+        <v>1347.899</v>
+      </c>
+      <c r="AJ343" s="0">
+        <v>1267.883</v>
+      </c>
+      <c r="AK343" s="0">
+        <v>829.6157</v>
+      </c>
+      <c r="AL343" s="0">
+        <v>624.674</v>
+      </c>
+      <c r="AM343" s="0">
+        <v>1093.788</v>
+      </c>
+      <c r="AN343" s="0">
+        <v>171.2757</v>
+      </c>
+      <c r="AO343" s="0">
+        <v>322.1214</v>
+      </c>
+      <c r="AP343" s="0">
+        <v>246.2144</v>
+      </c>
+      <c r="AQ343" s="0">
+        <v>121.2085</v>
+      </c>
+      <c r="AR343" s="0">
+        <v>108.2398</v>
+      </c>
+      <c r="AS343" s="0">
+        <v>706.2339</v>
+      </c>
+      <c r="AT343" s="0">
+        <v>787.6937</v>
+      </c>
+      <c r="AU343" s="0">
+        <v>399.2522</v>
+      </c>
+      <c r="AV343" s="0">
+        <v>825.0752</v>
+      </c>
+      <c r="AW343" s="0">
+        <v>224.2309</v>
+      </c>
+      <c r="AX343" s="0">
+        <v>687.1114</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="B344" s="0">
+        <v>303.8083</v>
+      </c>
+      <c r="C344" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D344" s="0">
+        <v>104.7949</v>
+      </c>
+      <c r="E344" s="0">
+        <v>157.3281</v>
+      </c>
+      <c r="F344" s="0">
+        <v>1125.615</v>
+      </c>
+      <c r="G344" s="0">
+        <v>342.8579</v>
+      </c>
+      <c r="H344" s="0">
+        <v>472.4969</v>
+      </c>
+      <c r="I344" s="0">
+        <v>260.7505</v>
+      </c>
+      <c r="J344" s="0">
+        <v>583.0536</v>
+      </c>
+      <c r="K344" s="0">
+        <v>771.4927</v>
+      </c>
+      <c r="L344" s="0">
+        <v>431.7147</v>
+      </c>
+      <c r="M344" s="0">
+        <v>1080.232</v>
+      </c>
+      <c r="N344" s="0">
+        <v>326.903</v>
+      </c>
+      <c r="O344" s="0">
+        <v>226.8498</v>
+      </c>
+      <c r="P344" s="0">
+        <v>234.3798</v>
+      </c>
+      <c r="Q344" s="0">
+        <v>270.7432</v>
+      </c>
+      <c r="R344" s="0">
+        <v>168.0424</v>
+      </c>
+      <c r="S344" s="0">
+        <v>321.7493</v>
+      </c>
+      <c r="T344" s="0">
+        <v>325.347</v>
+      </c>
+      <c r="U344" s="0">
+        <v>342.5222</v>
+      </c>
+      <c r="V344" s="0">
+        <v>265.5774</v>
+      </c>
+      <c r="W344" s="0">
+        <v>110.0165</v>
+      </c>
+      <c r="X344" s="0">
+        <v>211.4246</v>
+      </c>
+      <c r="Y344" s="0">
+        <v>680.4315</v>
+      </c>
+      <c r="Z344" s="0">
+        <v>473.4151</v>
+      </c>
+      <c r="AA344" s="0">
+        <v>235.5292</v>
+      </c>
+      <c r="AB344" s="0">
+        <v>178.863</v>
+      </c>
+      <c r="AC344" s="0">
+        <v>127.4801</v>
+      </c>
+      <c r="AD344" s="0">
+        <v>662.1352</v>
+      </c>
+      <c r="AE344" s="0">
+        <v>515.8236</v>
+      </c>
+      <c r="AF344" s="0">
+        <v>396.9666</v>
+      </c>
+      <c r="AG344" s="0">
+        <v>165.0533</v>
+      </c>
+      <c r="AH344" s="0">
+        <v>316.624</v>
+      </c>
+      <c r="AI344" s="0">
+        <v>1356.562</v>
+      </c>
+      <c r="AJ344" s="0">
+        <v>1275.499</v>
+      </c>
+      <c r="AK344" s="0">
+        <v>829.552</v>
+      </c>
+      <c r="AL344" s="0">
+        <v>625.8205</v>
+      </c>
+      <c r="AM344" s="0">
+        <v>1099.029</v>
+      </c>
+      <c r="AN344" s="0">
+        <v>168.8714</v>
+      </c>
+      <c r="AO344" s="0">
+        <v>319.8858</v>
+      </c>
+      <c r="AP344" s="0">
+        <v>246.6411</v>
+      </c>
+      <c r="AQ344" s="0">
+        <v>120.5704</v>
+      </c>
+      <c r="AR344" s="0">
+        <v>107.8783</v>
+      </c>
+      <c r="AS344" s="0">
+        <v>697.7741</v>
+      </c>
+      <c r="AT344" s="0">
+        <v>791.607</v>
+      </c>
+      <c r="AU344" s="0">
+        <v>405.1164</v>
+      </c>
+      <c r="AV344" s="0">
+        <v>829.148</v>
+      </c>
+      <c r="AW344" s="0">
+        <v>224.2347</v>
+      </c>
+      <c r="AX344" s="0">
+        <v>688.4308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the external macro data
</commit_message>
<xml_diff>
--- a/data-input/wb-data/global-economic-monitor/Emerging Market Bond Index (JPM Total Return Index).xlsx
+++ b/data-input/wb-data/global-economic-monitor/Emerging Market Bond Index (JPM Total Return Index).xlsx
@@ -5,14 +5,14 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="annual" sheetId="1" r:id="Rc6b6e846b44d410c"/>
-    <sheet name="monthly" sheetId="2" r:id="Rb27a24ce0bcd4593"/>
+    <sheet name="annual" sheetId="1" r:id="Rd2c71305527a4999"/>
+    <sheet name="monthly" sheetId="2" r:id="Re0b33552d30e4740"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="380">
   <si>
     <t/>
   </si>
@@ -1153,81 +1153,6 @@
   <si>
     <t>2017M05</t>
   </si>
-  <si>
-    <t>2017M06</t>
-  </si>
-  <si>
-    <t>2017M07</t>
-  </si>
-  <si>
-    <t>2017M08</t>
-  </si>
-  <si>
-    <t>2017M09</t>
-  </si>
-  <si>
-    <t>2017M10</t>
-  </si>
-  <si>
-    <t>2017M11</t>
-  </si>
-  <si>
-    <t>2017M12</t>
-  </si>
-  <si>
-    <t>2018M01</t>
-  </si>
-  <si>
-    <t>2018M02</t>
-  </si>
-  <si>
-    <t>2018M03</t>
-  </si>
-  <si>
-    <t>2018M04</t>
-  </si>
-  <si>
-    <t>2018M05</t>
-  </si>
-  <si>
-    <t>2018M06</t>
-  </si>
-  <si>
-    <t>2018M07</t>
-  </si>
-  <si>
-    <t>2018M08</t>
-  </si>
-  <si>
-    <t>2018M09</t>
-  </si>
-  <si>
-    <t>2018M10</t>
-  </si>
-  <si>
-    <t>2018M11</t>
-  </si>
-  <si>
-    <t>2018M12</t>
-  </si>
-  <si>
-    <t>2019M01</t>
-  </si>
-  <si>
-    <t>2019M02</t>
-  </si>
-  <si>
-    <t>2019M03</t>
-  </si>
-  <si>
-    <t>2019M04</t>
-  </si>
-  <si>
-    <t>2019M05</t>
-  </si>
-  <si>
-    <t>2019M06</t>
-  </si>
 </sst>
 </file>
 
@@ -1272,7 +1197,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AX32"/>
+  <dimension ref="A1:AX30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5691,455 +5616,151 @@
         <v>2017</v>
       </c>
       <c r="B30" s="0">
-        <v>312.4403</v>
+        <v>298.7677</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="0">
-        <v>102.5118</v>
+      <c r="D30" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="E30" s="0">
-        <v>145.696</v>
+        <v>133.02</v>
       </c>
       <c r="F30" s="0">
-        <v>1141.895</v>
+        <v>1110.006</v>
       </c>
       <c r="G30" s="0">
-        <v>346.8973</v>
+        <v>338.0221</v>
       </c>
       <c r="H30" s="0">
-        <v>474.5639</v>
+        <v>467.2907</v>
       </c>
       <c r="I30" s="0">
-        <v>257.0055</v>
+        <v>246.1352</v>
       </c>
       <c r="J30" s="0">
-        <v>582.0092</v>
+        <v>567.5512</v>
       </c>
       <c r="K30" s="0">
-        <v>784.5871</v>
+        <v>765.4304</v>
       </c>
       <c r="L30" s="0">
-        <v>431.8997</v>
+        <v>413.2959</v>
       </c>
       <c r="M30" s="0">
-        <v>1051.04</v>
+        <v>1010.05</v>
       </c>
       <c r="N30" s="0">
-        <v>319.1761</v>
+        <v>307.6356</v>
       </c>
       <c r="O30" s="0">
-        <v>218.3362</v>
+        <v>211.2394</v>
       </c>
       <c r="P30" s="0">
-        <v>232.0438</v>
+        <v>226.2743</v>
       </c>
       <c r="Q30" s="0">
-        <v>246.6009</v>
+        <v>231.5121</v>
       </c>
       <c r="R30" s="0">
-        <v>166.531</v>
+        <v>162.4309</v>
       </c>
       <c r="S30" s="0">
-        <v>323.1576</v>
+        <v>315.7248</v>
       </c>
       <c r="T30" s="0">
-        <v>330.0967</v>
+        <v>320.244</v>
       </c>
       <c r="U30" s="0">
-        <v>314.2443</v>
+        <v>296.8212</v>
       </c>
       <c r="V30" s="0">
-        <v>261.877</v>
+        <v>250.2176</v>
       </c>
       <c r="W30" s="0">
-        <v>112.3001</v>
+        <v>109.2859</v>
       </c>
       <c r="X30" s="0">
-        <v>207.0883</v>
+        <v>201.0759</v>
       </c>
       <c r="Y30" s="0">
-        <v>700.1031</v>
+        <v>682.7226</v>
       </c>
       <c r="Z30" s="0">
-        <v>506.4694</v>
+        <v>504.0743</v>
       </c>
       <c r="AA30" s="0">
-        <v>238.1539</v>
+        <v>230.012</v>
       </c>
       <c r="AB30" s="0">
-        <v>178.8438</v>
+        <v>176.3506</v>
       </c>
       <c r="AC30" s="0">
-        <v>128.8848</v>
+        <v>125.1186</v>
       </c>
       <c r="AD30" s="0">
-        <v>673.2803</v>
+        <v>648.711</v>
       </c>
       <c r="AE30" s="0">
-        <v>531.0272</v>
+        <v>524.4887</v>
       </c>
       <c r="AF30" s="0">
-        <v>398.6465</v>
+        <v>390.5243</v>
       </c>
       <c r="AG30" s="0">
-        <v>162.1726</v>
+        <v>155.9599</v>
       </c>
       <c r="AH30" s="0">
-        <v>320.4919</v>
+        <v>315.3009</v>
       </c>
       <c r="AI30" s="0">
-        <v>1359.7</v>
+        <v>1317.281</v>
       </c>
       <c r="AJ30" s="0">
-        <v>1289.767</v>
+        <v>1249.478</v>
       </c>
       <c r="AK30" s="0">
-        <v>853.5987</v>
+        <v>838.776</v>
       </c>
       <c r="AL30" s="0">
-        <v>628.5354</v>
+        <v>616.713</v>
       </c>
       <c r="AM30" s="0">
-        <v>1116.187</v>
+        <v>1100.546</v>
       </c>
       <c r="AN30" s="0">
-        <v>174.4722</v>
+        <v>167.3998</v>
       </c>
       <c r="AO30" s="0">
-        <v>292.571</v>
+        <v>275.9091</v>
       </c>
       <c r="AP30" s="0">
-        <v>244.3111</v>
+        <v>239.3408</v>
       </c>
       <c r="AQ30" s="0">
-        <v>117.3912</v>
+        <v>114.6746</v>
       </c>
       <c r="AR30" s="0">
-        <v>109.3469</v>
+        <v>106.2017</v>
       </c>
       <c r="AS30" s="0">
-        <v>739.2591</v>
+        <v>715.4025</v>
       </c>
       <c r="AT30" s="0">
-        <v>743.8789</v>
+        <v>700.0611</v>
       </c>
       <c r="AU30" s="0">
-        <v>401.603</v>
+        <v>380.783</v>
       </c>
       <c r="AV30" s="0">
-        <v>1171.342</v>
+        <v>1301.833</v>
       </c>
       <c r="AW30" s="0">
-        <v>222.018</v>
+        <v>215.7606</v>
       </c>
       <c r="AX30" s="0">
-        <v>681.5104</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="0">
-        <v>2018</v>
-      </c>
-      <c r="B31" s="0">
-        <v>294.7209</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="0">
-        <v>104.9447</v>
-      </c>
-      <c r="E31" s="0">
-        <v>157.2295</v>
-      </c>
-      <c r="F31" s="0">
-        <v>1160.028</v>
-      </c>
-      <c r="G31" s="0">
-        <v>346.6984</v>
-      </c>
-      <c r="H31" s="0">
-        <v>474.9429</v>
-      </c>
-      <c r="I31" s="0">
-        <v>262.1827</v>
-      </c>
-      <c r="J31" s="0">
-        <v>590.9561</v>
-      </c>
-      <c r="K31" s="0">
-        <v>778.0122</v>
-      </c>
-      <c r="L31" s="0">
-        <v>440.6091</v>
-      </c>
-      <c r="M31" s="0">
-        <v>1100.637</v>
-      </c>
-      <c r="N31" s="0">
-        <v>327.0217</v>
-      </c>
-      <c r="O31" s="0">
-        <v>225.2666</v>
-      </c>
-      <c r="P31" s="0">
-        <v>238.6115</v>
-      </c>
-      <c r="Q31" s="0">
-        <v>270.4382</v>
-      </c>
-      <c r="R31" s="0">
-        <v>170.2777</v>
-      </c>
-      <c r="S31" s="0">
-        <v>325.1717</v>
-      </c>
-      <c r="T31" s="0">
-        <v>329.4341</v>
-      </c>
-      <c r="U31" s="0">
-        <v>344.6378</v>
-      </c>
-      <c r="V31" s="0">
-        <v>272.3856</v>
-      </c>
-      <c r="W31" s="0">
-        <v>113.7077</v>
-      </c>
-      <c r="X31" s="0">
-        <v>214.5893</v>
-      </c>
-      <c r="Y31" s="0">
-        <v>685.5966</v>
-      </c>
-      <c r="Z31" s="0">
-        <v>484.5966</v>
-      </c>
-      <c r="AA31" s="0">
-        <v>236.1186</v>
-      </c>
-      <c r="AB31" s="0">
-        <v>180.3351</v>
-      </c>
-      <c r="AC31" s="0">
-        <v>129.5219</v>
-      </c>
-      <c r="AD31" s="0">
-        <v>674.0419</v>
-      </c>
-      <c r="AE31" s="0">
-        <v>523.1948</v>
-      </c>
-      <c r="AF31" s="0">
-        <v>400.9914</v>
-      </c>
-      <c r="AG31" s="0">
-        <v>164.089</v>
-      </c>
-      <c r="AH31" s="0">
-        <v>320.9605</v>
-      </c>
-      <c r="AI31" s="0">
-        <v>1372.214</v>
-      </c>
-      <c r="AJ31" s="0">
-        <v>1296.146</v>
-      </c>
-      <c r="AK31" s="0">
-        <v>842.0234</v>
-      </c>
-      <c r="AL31" s="0">
-        <v>631.0187</v>
-      </c>
-      <c r="AM31" s="0">
-        <v>1110.377</v>
-      </c>
-      <c r="AN31" s="0">
-        <v>172.1426</v>
-      </c>
-      <c r="AO31" s="0">
-        <v>322.3621</v>
-      </c>
-      <c r="AP31" s="0">
-        <v>248.9658</v>
-      </c>
-      <c r="AQ31" s="0">
-        <v>120.5735</v>
-      </c>
-      <c r="AR31" s="0">
-        <v>107.9301</v>
-      </c>
-      <c r="AS31" s="0">
-        <v>707.2581</v>
-      </c>
-      <c r="AT31" s="0">
-        <v>788.0752</v>
-      </c>
-      <c r="AU31" s="0">
-        <v>411.1503</v>
-      </c>
-      <c r="AV31" s="0">
-        <v>772.1309</v>
-      </c>
-      <c r="AW31" s="0">
-        <v>226.6539</v>
-      </c>
-      <c r="AX31" s="0">
-        <v>686.484</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="0">
-        <v>2019</v>
-      </c>
-      <c r="B32" s="0">
-        <v>275.1768</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="0">
-        <v>110.7685</v>
-      </c>
-      <c r="E32" s="0">
-        <v>167.2253</v>
-      </c>
-      <c r="F32" s="0">
-        <v>1262.231</v>
-      </c>
-      <c r="G32" s="0">
-        <v>369.6871</v>
-      </c>
-      <c r="H32" s="0">
-        <v>499.3428</v>
-      </c>
-      <c r="I32" s="0">
-        <v>274.5044</v>
-      </c>
-      <c r="J32" s="0">
-        <v>628.6858</v>
-      </c>
-      <c r="K32" s="0">
-        <v>816.1007</v>
-      </c>
-      <c r="L32" s="0">
-        <v>469.4519</v>
-      </c>
-      <c r="M32" s="0">
-        <v>1217.166</v>
-      </c>
-      <c r="N32" s="0">
-        <v>341.7759</v>
-      </c>
-      <c r="O32" s="0">
-        <v>240.0938</v>
-      </c>
-      <c r="P32" s="0">
-        <v>249.5265</v>
-      </c>
-      <c r="Q32" s="0">
-        <v>280.6078</v>
-      </c>
-      <c r="R32" s="0">
-        <v>178.6801</v>
-      </c>
-      <c r="S32" s="0">
-        <v>342.0721</v>
-      </c>
-      <c r="T32" s="0">
-        <v>351.8742</v>
-      </c>
-      <c r="U32" s="0">
-        <v>367.8577</v>
-      </c>
-      <c r="V32" s="0">
-        <v>289.9763</v>
-      </c>
-      <c r="W32" s="0">
-        <v>121.5764</v>
-      </c>
-      <c r="X32" s="0">
-        <v>231.6824</v>
-      </c>
-      <c r="Y32" s="0">
-        <v>715.5905</v>
-      </c>
-      <c r="Z32" s="0">
-        <v>490.0225</v>
-      </c>
-      <c r="AA32" s="0">
-        <v>245.7028</v>
-      </c>
-      <c r="AB32" s="0">
-        <v>185.6871</v>
-      </c>
-      <c r="AC32" s="0">
-        <v>135.6402</v>
-      </c>
-      <c r="AD32" s="0">
-        <v>697.8054</v>
-      </c>
-      <c r="AE32" s="0">
-        <v>536.6631</v>
-      </c>
-      <c r="AF32" s="0">
-        <v>423.0542</v>
-      </c>
-      <c r="AG32" s="0">
-        <v>172.5288</v>
-      </c>
-      <c r="AH32" s="0">
-        <v>350.4151</v>
-      </c>
-      <c r="AI32" s="0">
-        <v>1468.885</v>
-      </c>
-      <c r="AJ32" s="0">
-        <v>1403.996</v>
-      </c>
-      <c r="AK32" s="0">
-        <v>907.3552</v>
-      </c>
-      <c r="AL32" s="0">
-        <v>659.5287</v>
-      </c>
-      <c r="AM32" s="0">
-        <v>1178.014</v>
-      </c>
-      <c r="AN32" s="0">
-        <v>182.6983</v>
-      </c>
-      <c r="AO32" s="0">
-        <v>344.462</v>
-      </c>
-      <c r="AP32" s="0">
-        <v>258.3784</v>
-      </c>
-      <c r="AQ32" s="0">
-        <v>124.7224</v>
-      </c>
-      <c r="AR32" s="0">
-        <v>111.2699</v>
-      </c>
-      <c r="AS32" s="0">
-        <v>727.4245</v>
-      </c>
-      <c r="AT32" s="0">
-        <v>818.3938</v>
-      </c>
-      <c r="AU32" s="0">
-        <v>439.6663</v>
-      </c>
-      <c r="AV32" s="0">
-        <v>813.6907</v>
-      </c>
-      <c r="AW32" s="0">
-        <v>240.7852</v>
-      </c>
-      <c r="AX32" s="0">
-        <v>729.0773</v>
+        <v>672.6618</v>
       </c>
     </row>
   </sheetData>
@@ -6149,7 +5770,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AX356"/>
+  <dimension ref="A1:AX331"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -56320,7 +55941,7 @@
         <v>379</v>
       </c>
       <c r="B331" s="0">
-        <v>310.3837</v>
+        <v>310.1862</v>
       </c>
       <c r="C331" s="0" t="s">
         <v>50</v>
@@ -56329,3942 +55950,142 @@
         <v>50</v>
       </c>
       <c r="E331" s="0">
-        <v>155.8646</v>
+        <v>156.7992</v>
       </c>
       <c r="F331" s="0">
-        <v>1131.676</v>
+        <v>1132.338</v>
       </c>
       <c r="G331" s="0">
-        <v>343.5542</v>
+        <v>343.1394</v>
       </c>
       <c r="H331" s="0">
-        <v>471.8525</v>
+        <v>471.5216</v>
       </c>
       <c r="I331" s="0">
-        <v>253.3455</v>
+        <v>253.1732</v>
       </c>
       <c r="J331" s="0">
-        <v>577.4392</v>
+        <v>577.11</v>
       </c>
       <c r="K331" s="0">
-        <v>782.2889</v>
+        <v>781.5562</v>
       </c>
       <c r="L331" s="0">
-        <v>426.1649</v>
+        <v>425.8223</v>
       </c>
       <c r="M331" s="0">
-        <v>1017.225</v>
+        <v>1016.976</v>
       </c>
       <c r="N331" s="0">
-        <v>315.6239</v>
+        <v>315.6637</v>
       </c>
       <c r="O331" s="0">
-        <v>219.8637</v>
+        <v>219.5178</v>
       </c>
       <c r="P331" s="0">
-        <v>229.5309</v>
+        <v>229.3731</v>
       </c>
       <c r="Q331" s="0">
-        <v>238.0465</v>
+        <v>237.2408</v>
       </c>
       <c r="R331" s="0">
-        <v>164.5896</v>
+        <v>164.4323</v>
       </c>
       <c r="S331" s="0">
-        <v>320.5753</v>
+        <v>320.3796</v>
       </c>
       <c r="T331" s="0">
-        <v>326.5907</v>
+        <v>326.1968</v>
       </c>
       <c r="U331" s="0">
-        <v>310.6251</v>
+        <v>309.6959</v>
       </c>
       <c r="V331" s="0">
-        <v>257.6955</v>
+        <v>257.2084</v>
       </c>
       <c r="W331" s="0">
-        <v>112.1303</v>
+        <v>112.0204</v>
       </c>
       <c r="X331" s="0">
-        <v>204.5221</v>
+        <v>204.3424</v>
       </c>
       <c r="Y331" s="0">
-        <v>700.2286</v>
+        <v>699.5479</v>
       </c>
       <c r="Z331" s="0">
-        <v>513.4411</v>
+        <v>513.6075</v>
       </c>
       <c r="AA331" s="0">
-        <v>235.776</v>
+        <v>235.6486</v>
       </c>
       <c r="AB331" s="0">
-        <v>178.3555</v>
+        <v>178.2993</v>
       </c>
       <c r="AC331" s="0">
-        <v>128.0544</v>
+        <v>127.9149</v>
       </c>
       <c r="AD331" s="0">
-        <v>671.0194</v>
+        <v>670.4325</v>
       </c>
       <c r="AE331" s="0">
-        <v>535.8772</v>
+        <v>535.6836</v>
       </c>
       <c r="AF331" s="0">
-        <v>394.6023</v>
+        <v>394.256</v>
       </c>
       <c r="AG331" s="0">
-        <v>161.6575</v>
+        <v>161.3862</v>
       </c>
       <c r="AH331" s="0">
-        <v>318.7653</v>
+        <v>318.6147</v>
       </c>
       <c r="AI331" s="0">
-        <v>1343.885</v>
+        <v>1342.772</v>
       </c>
       <c r="AJ331" s="0">
-        <v>1276.46</v>
+        <v>1274.782</v>
       </c>
       <c r="AK331" s="0">
-        <v>846.7976</v>
+        <v>846.4003</v>
       </c>
       <c r="AL331" s="0">
-        <v>625.0639</v>
+        <v>624.4434</v>
       </c>
       <c r="AM331" s="0">
-        <v>1115.307</v>
+        <v>1114.632</v>
       </c>
       <c r="AN331" s="0">
-        <v>173.351</v>
+        <v>173.0445</v>
       </c>
       <c r="AO331" s="0">
-        <v>279.2232</v>
+        <v>278.8592</v>
       </c>
       <c r="AP331" s="0">
-        <v>242.9449</v>
+        <v>242.8337</v>
       </c>
       <c r="AQ331" s="0">
-        <v>115.3255</v>
+        <v>115.2755</v>
       </c>
       <c r="AR331" s="0">
-        <v>109.1092</v>
+        <v>109.265</v>
       </c>
       <c r="AS331" s="0">
-        <v>743.1958</v>
+        <v>742.0132</v>
       </c>
       <c r="AT331" s="0">
-        <v>727.2636</v>
+        <v>726.1553</v>
       </c>
       <c r="AU331" s="0">
-        <v>391.4898</v>
+        <v>390.9775</v>
       </c>
       <c r="AV331" s="0">
-        <v>1314.352</v>
+        <v>1308.952</v>
       </c>
       <c r="AW331" s="0">
-        <v>219.5223</v>
+        <v>219.3083</v>
       </c>
       <c r="AX331" s="0">
-        <v>680.6609</v>
-      </c>
-    </row>
-    <row r="332">
-      <c r="A332" s="0" t="s">
-        <v>380</v>
-      </c>
-      <c r="B332" s="0">
-        <v>313.2231</v>
-      </c>
-      <c r="C332" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D332" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E332" s="0">
-        <v>150.3216</v>
-      </c>
-      <c r="F332" s="0">
-        <v>1131.757</v>
-      </c>
-      <c r="G332" s="0">
-        <v>348.7304</v>
-      </c>
-      <c r="H332" s="0">
-        <v>475.789</v>
-      </c>
-      <c r="I332" s="0">
-        <v>256.5779</v>
-      </c>
-      <c r="J332" s="0">
-        <v>585.9471</v>
-      </c>
-      <c r="K332" s="0">
-        <v>789.0706</v>
-      </c>
-      <c r="L332" s="0">
-        <v>432.8783</v>
-      </c>
-      <c r="M332" s="0">
-        <v>1009.299</v>
-      </c>
-      <c r="N332" s="0">
-        <v>315.2223</v>
-      </c>
-      <c r="O332" s="0">
-        <v>220.0537</v>
-      </c>
-      <c r="P332" s="0">
-        <v>231.3503</v>
-      </c>
-      <c r="Q332" s="0">
-        <v>245.027</v>
-      </c>
-      <c r="R332" s="0">
-        <v>167.1934</v>
-      </c>
-      <c r="S332" s="0">
-        <v>324.4161</v>
-      </c>
-      <c r="T332" s="0">
-        <v>331.271</v>
-      </c>
-      <c r="U332" s="0">
-        <v>312.4435</v>
-      </c>
-      <c r="V332" s="0">
-        <v>261.6836</v>
-      </c>
-      <c r="W332" s="0">
-        <v>113.3755</v>
-      </c>
-      <c r="X332" s="0">
-        <v>206.2913</v>
-      </c>
-      <c r="Y332" s="0">
-        <v>705.4266</v>
-      </c>
-      <c r="Z332" s="0">
-        <v>514.0635</v>
-      </c>
-      <c r="AA332" s="0">
-        <v>237.6132</v>
-      </c>
-      <c r="AB332" s="0">
-        <v>179.7725</v>
-      </c>
-      <c r="AC332" s="0">
-        <v>129.8512</v>
-      </c>
-      <c r="AD332" s="0">
-        <v>679.6829</v>
-      </c>
-      <c r="AE332" s="0">
-        <v>535.6541</v>
-      </c>
-      <c r="AF332" s="0">
-        <v>399.8843</v>
-      </c>
-      <c r="AG332" s="0">
-        <v>162.2367</v>
-      </c>
-      <c r="AH332" s="0">
-        <v>323.1272</v>
-      </c>
-      <c r="AI332" s="0">
-        <v>1361.812</v>
-      </c>
-      <c r="AJ332" s="0">
-        <v>1296.477</v>
-      </c>
-      <c r="AK332" s="0">
-        <v>859.2395</v>
-      </c>
-      <c r="AL332" s="0">
-        <v>634.8366</v>
-      </c>
-      <c r="AM332" s="0">
-        <v>1117.385</v>
-      </c>
-      <c r="AN332" s="0">
-        <v>174.9762</v>
-      </c>
-      <c r="AO332" s="0">
-        <v>285.3675</v>
-      </c>
-      <c r="AP332" s="0">
-        <v>245.4975</v>
-      </c>
-      <c r="AQ332" s="0">
-        <v>115.6137</v>
-      </c>
-      <c r="AR332" s="0">
-        <v>108.6509</v>
-      </c>
-      <c r="AS332" s="0">
-        <v>753.0497</v>
-      </c>
-      <c r="AT332" s="0">
-        <v>737.5254</v>
-      </c>
-      <c r="AU332" s="0">
-        <v>403.1338</v>
-      </c>
-      <c r="AV332" s="0">
-        <v>1266.312</v>
-      </c>
-      <c r="AW332" s="0">
-        <v>222.4599</v>
-      </c>
-      <c r="AX332" s="0">
-        <v>684.5675</v>
-      </c>
-    </row>
-    <row r="333">
-      <c r="A333" s="0" t="s">
-        <v>381</v>
-      </c>
-      <c r="B333" s="0">
-        <v>307.0583</v>
-      </c>
-      <c r="C333" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D333" s="0">
-        <v>100</v>
-      </c>
-      <c r="E333" s="0">
-        <v>151.72</v>
-      </c>
-      <c r="F333" s="0">
-        <v>1138.9</v>
-      </c>
-      <c r="G333" s="0">
-        <v>347.9345</v>
-      </c>
-      <c r="H333" s="0">
-        <v>475.3736</v>
-      </c>
-      <c r="I333" s="0">
-        <v>256.6299</v>
-      </c>
-      <c r="J333" s="0">
-        <v>580.3979</v>
-      </c>
-      <c r="K333" s="0">
-        <v>786.2865</v>
-      </c>
-      <c r="L333" s="0">
-        <v>433.8236</v>
-      </c>
-      <c r="M333" s="0">
-        <v>1025.562</v>
-      </c>
-      <c r="N333" s="0">
-        <v>317.5771</v>
-      </c>
-      <c r="O333" s="0">
-        <v>215.4965</v>
-      </c>
-      <c r="P333" s="0">
-        <v>231.4337</v>
-      </c>
-      <c r="Q333" s="0">
-        <v>245.3899</v>
-      </c>
-      <c r="R333" s="0">
-        <v>167.4078</v>
-      </c>
-      <c r="S333" s="0">
-        <v>324.0184</v>
-      </c>
-      <c r="T333" s="0">
-        <v>330.8118</v>
-      </c>
-      <c r="U333" s="0">
-        <v>310.6144</v>
-      </c>
-      <c r="V333" s="0">
-        <v>262.0889</v>
-      </c>
-      <c r="W333" s="0">
-        <v>112.58</v>
-      </c>
-      <c r="X333" s="0">
-        <v>204.3799</v>
-      </c>
-      <c r="Y333" s="0">
-        <v>702.0415</v>
-      </c>
-      <c r="Z333" s="0">
-        <v>509.1174</v>
-      </c>
-      <c r="AA333" s="0">
-        <v>237.8685</v>
-      </c>
-      <c r="AB333" s="0">
-        <v>179.3239</v>
-      </c>
-      <c r="AC333" s="0">
-        <v>129.5332</v>
-      </c>
-      <c r="AD333" s="0">
-        <v>678.7455</v>
-      </c>
-      <c r="AE333" s="0">
-        <v>532.0757</v>
-      </c>
-      <c r="AF333" s="0">
-        <v>399.7633</v>
-      </c>
-      <c r="AG333" s="0">
-        <v>162.3641</v>
-      </c>
-      <c r="AH333" s="0">
-        <v>321.1906</v>
-      </c>
-      <c r="AI333" s="0">
-        <v>1360.771</v>
-      </c>
-      <c r="AJ333" s="0">
-        <v>1289.852</v>
-      </c>
-      <c r="AK333" s="0">
-        <v>856.9716</v>
-      </c>
-      <c r="AL333" s="0">
-        <v>631.0704</v>
-      </c>
-      <c r="AM333" s="0">
-        <v>1114.722</v>
-      </c>
-      <c r="AN333" s="0">
-        <v>175.0419</v>
-      </c>
-      <c r="AO333" s="0">
-        <v>286.1093</v>
-      </c>
-      <c r="AP333" s="0">
-        <v>245.7099</v>
-      </c>
-      <c r="AQ333" s="0">
-        <v>116.8208</v>
-      </c>
-      <c r="AR333" s="0">
-        <v>107.9678</v>
-      </c>
-      <c r="AS333" s="0">
-        <v>748.5402</v>
-      </c>
-      <c r="AT333" s="0">
-        <v>746.0607</v>
-      </c>
-      <c r="AU333" s="0">
-        <v>404.2867</v>
-      </c>
-      <c r="AV333" s="0">
-        <v>1224.792</v>
-      </c>
-      <c r="AW333" s="0">
-        <v>223.1732</v>
-      </c>
-      <c r="AX333" s="0">
-        <v>677.3122</v>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334" s="0" t="s">
-        <v>382</v>
-      </c>
-      <c r="B334" s="0">
-        <v>314.6261</v>
-      </c>
-      <c r="C334" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D334" s="0">
-        <v>101.1343</v>
-      </c>
-      <c r="E334" s="0">
-        <v>153.2755</v>
-      </c>
-      <c r="F334" s="0">
-        <v>1156.226</v>
-      </c>
-      <c r="G334" s="0">
-        <v>352.3483</v>
-      </c>
-      <c r="H334" s="0">
-        <v>479.8611</v>
-      </c>
-      <c r="I334" s="0">
-        <v>263.3813</v>
-      </c>
-      <c r="J334" s="0">
-        <v>587.5414</v>
-      </c>
-      <c r="K334" s="0">
-        <v>795.7098</v>
-      </c>
-      <c r="L334" s="0">
-        <v>444.1007</v>
-      </c>
-      <c r="M334" s="0">
-        <v>1059.226</v>
-      </c>
-      <c r="N334" s="0">
-        <v>324.7193</v>
-      </c>
-      <c r="O334" s="0">
-        <v>221.8748</v>
-      </c>
-      <c r="P334" s="0">
-        <v>233.5368</v>
-      </c>
-      <c r="Q334" s="0">
-        <v>253.2651</v>
-      </c>
-      <c r="R334" s="0">
-        <v>169.2409</v>
-      </c>
-      <c r="S334" s="0">
-        <v>327.9945</v>
-      </c>
-      <c r="T334" s="0">
-        <v>335.6142</v>
-      </c>
-      <c r="U334" s="0">
-        <v>328.4086</v>
-      </c>
-      <c r="V334" s="0">
-        <v>266.4472</v>
-      </c>
-      <c r="W334" s="0">
-        <v>114.2727</v>
-      </c>
-      <c r="X334" s="0">
-        <v>209.1574</v>
-      </c>
-      <c r="Y334" s="0">
-        <v>708.2351</v>
-      </c>
-      <c r="Z334" s="0">
-        <v>511.7914</v>
-      </c>
-      <c r="AA334" s="0">
-        <v>243.4078</v>
-      </c>
-      <c r="AB334" s="0">
-        <v>180.1339</v>
-      </c>
-      <c r="AC334" s="0">
-        <v>131.9034</v>
-      </c>
-      <c r="AD334" s="0">
-        <v>690.1185</v>
-      </c>
-      <c r="AE334" s="0">
-        <v>537.99</v>
-      </c>
-      <c r="AF334" s="0">
-        <v>402.4234</v>
-      </c>
-      <c r="AG334" s="0">
-        <v>165.9736</v>
-      </c>
-      <c r="AH334" s="0">
-        <v>323.8704</v>
-      </c>
-      <c r="AI334" s="0">
-        <v>1379.818</v>
-      </c>
-      <c r="AJ334" s="0">
-        <v>1310.601</v>
-      </c>
-      <c r="AK334" s="0">
-        <v>864.8444</v>
-      </c>
-      <c r="AL334" s="0">
-        <v>637.0279</v>
-      </c>
-      <c r="AM334" s="0">
-        <v>1125.392</v>
-      </c>
-      <c r="AN334" s="0">
-        <v>177.9641</v>
-      </c>
-      <c r="AO334" s="0">
-        <v>291.8276</v>
-      </c>
-      <c r="AP334" s="0">
-        <v>248.0173</v>
-      </c>
-      <c r="AQ334" s="0">
-        <v>119.0266</v>
-      </c>
-      <c r="AR334" s="0">
-        <v>110.7102</v>
-      </c>
-      <c r="AS334" s="0">
-        <v>764.4388</v>
-      </c>
-      <c r="AT334" s="0">
-        <v>760.1128</v>
-      </c>
-      <c r="AU334" s="0">
-        <v>411.2404</v>
-      </c>
-      <c r="AV334" s="0">
-        <v>1112.674</v>
-      </c>
-      <c r="AW334" s="0">
-        <v>225.1702</v>
-      </c>
-      <c r="AX334" s="0">
-        <v>688.8903</v>
-      </c>
-    </row>
-    <row r="335">
-      <c r="A335" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="B335" s="0">
-        <v>325.7467</v>
-      </c>
-      <c r="C335" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D335" s="0">
-        <v>103.2158</v>
-      </c>
-      <c r="E335" s="0">
-        <v>158.7616</v>
-      </c>
-      <c r="F335" s="0">
-        <v>1173.075</v>
-      </c>
-      <c r="G335" s="0">
-        <v>354.9358</v>
-      </c>
-      <c r="H335" s="0">
-        <v>482.1215</v>
-      </c>
-      <c r="I335" s="0">
-        <v>266.7595</v>
-      </c>
-      <c r="J335" s="0">
-        <v>596.2766</v>
-      </c>
-      <c r="K335" s="0">
-        <v>805.346</v>
-      </c>
-      <c r="L335" s="0">
-        <v>450.3855</v>
-      </c>
-      <c r="M335" s="0">
-        <v>1072.936</v>
-      </c>
-      <c r="N335" s="0">
-        <v>330.598</v>
-      </c>
-      <c r="O335" s="0">
-        <v>222.2829</v>
-      </c>
-      <c r="P335" s="0">
-        <v>237.2542</v>
-      </c>
-      <c r="Q335" s="0">
-        <v>258.1385</v>
-      </c>
-      <c r="R335" s="0">
-        <v>170.5593</v>
-      </c>
-      <c r="S335" s="0">
-        <v>331.2728</v>
-      </c>
-      <c r="T335" s="0">
-        <v>340.4071</v>
-      </c>
-      <c r="U335" s="0">
-        <v>328.9319</v>
-      </c>
-      <c r="V335" s="0">
-        <v>274.0704</v>
-      </c>
-      <c r="W335" s="0">
-        <v>114.6055</v>
-      </c>
-      <c r="X335" s="0">
-        <v>213.0669</v>
-      </c>
-      <c r="Y335" s="0">
-        <v>719.647</v>
-      </c>
-      <c r="Z335" s="0">
-        <v>514.7705</v>
-      </c>
-      <c r="AA335" s="0">
-        <v>246.6709</v>
-      </c>
-      <c r="AB335" s="0">
-        <v>181.0646</v>
-      </c>
-      <c r="AC335" s="0">
-        <v>133.1739</v>
-      </c>
-      <c r="AD335" s="0">
-        <v>698.9501</v>
-      </c>
-      <c r="AE335" s="0">
-        <v>540.771</v>
-      </c>
-      <c r="AF335" s="0">
-        <v>404.9827</v>
-      </c>
-      <c r="AG335" s="0">
-        <v>168.3679</v>
-      </c>
-      <c r="AH335" s="0">
-        <v>326.3869</v>
-      </c>
-      <c r="AI335" s="0">
-        <v>1403.79</v>
-      </c>
-      <c r="AJ335" s="0">
-        <v>1332.18</v>
-      </c>
-      <c r="AK335" s="0">
-        <v>871.1891</v>
-      </c>
-      <c r="AL335" s="0">
-        <v>640.2761</v>
-      </c>
-      <c r="AM335" s="0">
-        <v>1133.469</v>
-      </c>
-      <c r="AN335" s="0">
-        <v>180.2594</v>
-      </c>
-      <c r="AO335" s="0">
-        <v>304.5514</v>
-      </c>
-      <c r="AP335" s="0">
-        <v>248.737</v>
-      </c>
-      <c r="AQ335" s="0">
-        <v>120.145</v>
-      </c>
-      <c r="AR335" s="0">
-        <v>112.3723</v>
-      </c>
-      <c r="AS335" s="0">
-        <v>767.0001</v>
-      </c>
-      <c r="AT335" s="0">
-        <v>788.1268</v>
-      </c>
-      <c r="AU335" s="0">
-        <v>419.3093</v>
-      </c>
-      <c r="AV335" s="0">
-        <v>1115.689</v>
-      </c>
-      <c r="AW335" s="0">
-        <v>227.4769</v>
-      </c>
-      <c r="AX335" s="0">
-        <v>695.1902</v>
-      </c>
-    </row>
-    <row r="336">
-      <c r="A336" s="0" t="s">
-        <v>384</v>
-      </c>
-      <c r="B336" s="0">
-        <v>330.2703</v>
-      </c>
-      <c r="C336" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D336" s="0">
-        <v>103.7922</v>
-      </c>
-      <c r="E336" s="0">
-        <v>161.9452</v>
-      </c>
-      <c r="F336" s="0">
-        <v>1180.037</v>
-      </c>
-      <c r="G336" s="0">
-        <v>354.3815</v>
-      </c>
-      <c r="H336" s="0">
-        <v>481.942</v>
-      </c>
-      <c r="I336" s="0">
-        <v>267.4821</v>
-      </c>
-      <c r="J336" s="0">
-        <v>593.8723</v>
-      </c>
-      <c r="K336" s="0">
-        <v>804.6338</v>
-      </c>
-      <c r="L336" s="0">
-        <v>449.8513</v>
-      </c>
-      <c r="M336" s="0">
-        <v>1100.152</v>
-      </c>
-      <c r="N336" s="0">
-        <v>330.9285</v>
-      </c>
-      <c r="O336" s="0">
-        <v>224.1007</v>
-      </c>
-      <c r="P336" s="0">
-        <v>238.2426</v>
-      </c>
-      <c r="Q336" s="0">
-        <v>262.7612</v>
-      </c>
-      <c r="R336" s="0">
-        <v>170.2461</v>
-      </c>
-      <c r="S336" s="0">
-        <v>330.3672</v>
-      </c>
-      <c r="T336" s="0">
-        <v>340.4912</v>
-      </c>
-      <c r="U336" s="0">
-        <v>327.8767</v>
-      </c>
-      <c r="V336" s="0">
-        <v>275.6981</v>
-      </c>
-      <c r="W336" s="0">
-        <v>114.655</v>
-      </c>
-      <c r="X336" s="0">
-        <v>213.0492</v>
-      </c>
-      <c r="Y336" s="0">
-        <v>720.2223</v>
-      </c>
-      <c r="Z336" s="0">
-        <v>513.2567</v>
-      </c>
-      <c r="AA336" s="0">
-        <v>247.607</v>
-      </c>
-      <c r="AB336" s="0">
-        <v>181.2542</v>
-      </c>
-      <c r="AC336" s="0">
-        <v>131.6352</v>
-      </c>
-      <c r="AD336" s="0">
-        <v>692.3655</v>
-      </c>
-      <c r="AE336" s="0">
-        <v>539.2168</v>
-      </c>
-      <c r="AF336" s="0">
-        <v>406.0664</v>
-      </c>
-      <c r="AG336" s="0">
-        <v>166.8564</v>
-      </c>
-      <c r="AH336" s="0">
-        <v>326.3551</v>
-      </c>
-      <c r="AI336" s="0">
-        <v>1397.816</v>
-      </c>
-      <c r="AJ336" s="0">
-        <v>1324.361</v>
-      </c>
-      <c r="AK336" s="0">
-        <v>865.6678</v>
-      </c>
-      <c r="AL336" s="0">
-        <v>638.4602</v>
-      </c>
-      <c r="AM336" s="0">
-        <v>1129.901</v>
-      </c>
-      <c r="AN336" s="0">
-        <v>181.4841</v>
-      </c>
-      <c r="AO336" s="0">
-        <v>316.2143</v>
-      </c>
-      <c r="AP336" s="0">
-        <v>248.5766</v>
-      </c>
-      <c r="AQ336" s="0">
-        <v>120.2755</v>
-      </c>
-      <c r="AR336" s="0">
-        <v>112.3319</v>
-      </c>
-      <c r="AS336" s="0">
-        <v>757.8747</v>
-      </c>
-      <c r="AT336" s="0">
-        <v>793.3496</v>
-      </c>
-      <c r="AU336" s="0">
-        <v>419.7182</v>
-      </c>
-      <c r="AV336" s="0">
-        <v>1125.92</v>
-      </c>
-      <c r="AW336" s="0">
-        <v>228.7779</v>
-      </c>
-      <c r="AX336" s="0">
-        <v>689.7772</v>
-      </c>
-    </row>
-    <row r="337">
-      <c r="A337" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="B337" s="0">
-        <v>330.1189</v>
-      </c>
-      <c r="C337" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D337" s="0">
-        <v>102.645</v>
-      </c>
-      <c r="E337" s="0">
-        <v>155.1837</v>
-      </c>
-      <c r="F337" s="0">
-        <v>1181.904</v>
-      </c>
-      <c r="G337" s="0">
-        <v>355.4273</v>
-      </c>
-      <c r="H337" s="0">
-        <v>482.1311</v>
-      </c>
-      <c r="I337" s="0">
-        <v>269.063</v>
-      </c>
-      <c r="J337" s="0">
-        <v>596.8145</v>
-      </c>
-      <c r="K337" s="0">
-        <v>800.4916</v>
-      </c>
-      <c r="L337" s="0">
-        <v>450.8549</v>
-      </c>
-      <c r="M337" s="0">
-        <v>1123.759</v>
-      </c>
-      <c r="N337" s="0">
-        <v>334.8871</v>
-      </c>
-      <c r="O337" s="0">
-        <v>226.6121</v>
-      </c>
-      <c r="P337" s="0">
-        <v>239.6498</v>
-      </c>
-      <c r="Q337" s="0">
-        <v>265.5703</v>
-      </c>
-      <c r="R337" s="0">
-        <v>170.3487</v>
-      </c>
-      <c r="S337" s="0">
-        <v>330.0208</v>
-      </c>
-      <c r="T337" s="0">
-        <v>339.7941</v>
-      </c>
-      <c r="U337" s="0">
-        <v>335.2878</v>
-      </c>
-      <c r="V337" s="0">
-        <v>276.3206</v>
-      </c>
-      <c r="W337" s="0">
-        <v>114.9521</v>
-      </c>
-      <c r="X337" s="0">
-        <v>215.1184</v>
-      </c>
-      <c r="Y337" s="0">
-        <v>713.9695</v>
-      </c>
-      <c r="Z337" s="0">
-        <v>491.5568</v>
-      </c>
-      <c r="AA337" s="0">
-        <v>246.9454</v>
-      </c>
-      <c r="AB337" s="0">
-        <v>181.4357</v>
-      </c>
-      <c r="AC337" s="0">
-        <v>131.4185</v>
-      </c>
-      <c r="AD337" s="0">
-        <v>695.7638</v>
-      </c>
-      <c r="AE337" s="0">
-        <v>527.9686</v>
-      </c>
-      <c r="AF337" s="0">
-        <v>408.6856</v>
-      </c>
-      <c r="AG337" s="0">
-        <v>168.6006</v>
-      </c>
-      <c r="AH337" s="0">
-        <v>323.0053</v>
-      </c>
-      <c r="AI337" s="0">
-        <v>1410.213</v>
-      </c>
-      <c r="AJ337" s="0">
-        <v>1334.391</v>
-      </c>
-      <c r="AK337" s="0">
-        <v>864.2645</v>
-      </c>
-      <c r="AL337" s="0">
-        <v>637.945</v>
-      </c>
-      <c r="AM337" s="0">
-        <v>1132.887</v>
-      </c>
-      <c r="AN337" s="0">
-        <v>182.0162</v>
-      </c>
-      <c r="AO337" s="0">
-        <v>320.0802</v>
-      </c>
-      <c r="AP337" s="0">
-        <v>248.9659</v>
-      </c>
-      <c r="AQ337" s="0">
-        <v>121.0454</v>
-      </c>
-      <c r="AR337" s="0">
-        <v>114.1317</v>
-      </c>
-      <c r="AS337" s="0">
-        <v>743.1739</v>
-      </c>
-      <c r="AT337" s="0">
-        <v>797.6631</v>
-      </c>
-      <c r="AU337" s="0">
-        <v>426.0023</v>
-      </c>
-      <c r="AV337" s="0">
-        <v>881.6807</v>
-      </c>
-      <c r="AW337" s="0">
-        <v>228.8298</v>
-      </c>
-      <c r="AX337" s="0">
-        <v>682.5887</v>
-      </c>
-    </row>
-    <row r="338">
-      <c r="A338" s="0" t="s">
-        <v>386</v>
-      </c>
-      <c r="B338" s="0">
-        <v>334.2042</v>
-      </c>
-      <c r="C338" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D338" s="0">
-        <v>104.2834</v>
-      </c>
-      <c r="E338" s="0">
-        <v>152.9791</v>
-      </c>
-      <c r="F338" s="0">
-        <v>1191.469</v>
-      </c>
-      <c r="G338" s="0">
-        <v>358.4847</v>
-      </c>
-      <c r="H338" s="0">
-        <v>480.7642</v>
-      </c>
-      <c r="I338" s="0">
-        <v>273.3235</v>
-      </c>
-      <c r="J338" s="0">
-        <v>605.1751</v>
-      </c>
-      <c r="K338" s="0">
-        <v>805.6224</v>
-      </c>
-      <c r="L338" s="0">
-        <v>454.0797</v>
-      </c>
-      <c r="M338" s="0">
-        <v>1171.046</v>
-      </c>
-      <c r="N338" s="0">
-        <v>338.042</v>
-      </c>
-      <c r="O338" s="0">
-        <v>233.0704</v>
-      </c>
-      <c r="P338" s="0">
-        <v>241.5289</v>
-      </c>
-      <c r="Q338" s="0">
-        <v>270.6924</v>
-      </c>
-      <c r="R338" s="0">
-        <v>171.0644</v>
-      </c>
-      <c r="S338" s="0">
-        <v>330.9822</v>
-      </c>
-      <c r="T338" s="0">
-        <v>341.1567</v>
-      </c>
-      <c r="U338" s="0">
-        <v>342.3328</v>
-      </c>
-      <c r="V338" s="0">
-        <v>274.6393</v>
-      </c>
-      <c r="W338" s="0">
-        <v>116.6214</v>
-      </c>
-      <c r="X338" s="0">
-        <v>218.4371</v>
-      </c>
-      <c r="Y338" s="0">
-        <v>717.4021</v>
-      </c>
-      <c r="Z338" s="0">
-        <v>502.8719</v>
-      </c>
-      <c r="AA338" s="0">
-        <v>247.5469</v>
-      </c>
-      <c r="AB338" s="0">
-        <v>181.3321</v>
-      </c>
-      <c r="AC338" s="0">
-        <v>133.3699</v>
-      </c>
-      <c r="AD338" s="0">
-        <v>699.5957</v>
-      </c>
-      <c r="AE338" s="0">
-        <v>536.0125</v>
-      </c>
-      <c r="AF338" s="0">
-        <v>408.9845</v>
-      </c>
-      <c r="AG338" s="0">
-        <v>171.6015</v>
-      </c>
-      <c r="AH338" s="0">
-        <v>325.3126</v>
-      </c>
-      <c r="AI338" s="0">
-        <v>1414.664</v>
-      </c>
-      <c r="AJ338" s="0">
-        <v>1340.27</v>
-      </c>
-      <c r="AK338" s="0">
-        <v>866.7303</v>
-      </c>
-      <c r="AL338" s="0">
-        <v>638.6234</v>
-      </c>
-      <c r="AM338" s="0">
-        <v>1137.08</v>
-      </c>
-      <c r="AN338" s="0">
-        <v>184.6191</v>
-      </c>
-      <c r="AO338" s="0">
-        <v>326.7916</v>
-      </c>
-      <c r="AP338" s="0">
-        <v>249.4141</v>
-      </c>
-      <c r="AQ338" s="0">
-        <v>122.3439</v>
-      </c>
-      <c r="AR338" s="0">
-        <v>115.1453</v>
-      </c>
-      <c r="AS338" s="0">
-        <v>758.8371</v>
-      </c>
-      <c r="AT338" s="0">
-        <v>802.295</v>
-      </c>
-      <c r="AU338" s="0">
-        <v>431.118</v>
-      </c>
-      <c r="AV338" s="0">
-        <v>814.4782</v>
-      </c>
-      <c r="AW338" s="0">
-        <v>229.3115</v>
-      </c>
-      <c r="AX338" s="0">
-        <v>695.6531</v>
-      </c>
-    </row>
-    <row r="339">
-      <c r="A339" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="B339" s="0">
-        <v>330.0022</v>
-      </c>
-      <c r="C339" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D339" s="0">
-        <v>108.0205</v>
-      </c>
-      <c r="E339" s="0">
-        <v>152.4645</v>
-      </c>
-      <c r="F339" s="0">
-        <v>1194.814</v>
-      </c>
-      <c r="G339" s="0">
-        <v>357.1162</v>
-      </c>
-      <c r="H339" s="0">
-        <v>478.6045</v>
-      </c>
-      <c r="I339" s="0">
-        <v>278.2938</v>
-      </c>
-      <c r="J339" s="0">
-        <v>606.9312</v>
-      </c>
-      <c r="K339" s="0">
-        <v>807.852</v>
-      </c>
-      <c r="L339" s="0">
-        <v>458.1646</v>
-      </c>
-      <c r="M339" s="0">
-        <v>1178.353</v>
-      </c>
-      <c r="N339" s="0">
-        <v>342.1025</v>
-      </c>
-      <c r="O339" s="0">
-        <v>237.1826</v>
-      </c>
-      <c r="P339" s="0">
-        <v>241.7074</v>
-      </c>
-      <c r="Q339" s="0">
-        <v>274.8081</v>
-      </c>
-      <c r="R339" s="0">
-        <v>170.8917</v>
-      </c>
-      <c r="S339" s="0">
-        <v>329.3302</v>
-      </c>
-      <c r="T339" s="0">
-        <v>341.2853</v>
-      </c>
-      <c r="U339" s="0">
-        <v>351.3665</v>
-      </c>
-      <c r="V339" s="0">
-        <v>277.7983</v>
-      </c>
-      <c r="W339" s="0">
-        <v>118.5037</v>
-      </c>
-      <c r="X339" s="0">
-        <v>219.4301</v>
-      </c>
-      <c r="Y339" s="0">
-        <v>717.016</v>
-      </c>
-      <c r="Z339" s="0">
-        <v>519.7412</v>
-      </c>
-      <c r="AA339" s="0">
-        <v>248.4503</v>
-      </c>
-      <c r="AB339" s="0">
-        <v>180.4499</v>
-      </c>
-      <c r="AC339" s="0">
-        <v>134.1254</v>
-      </c>
-      <c r="AD339" s="0">
-        <v>697.7149</v>
-      </c>
-      <c r="AE339" s="0">
-        <v>546.7361</v>
-      </c>
-      <c r="AF339" s="0">
-        <v>407.7191</v>
-      </c>
-      <c r="AG339" s="0">
-        <v>174.3057</v>
-      </c>
-      <c r="AH339" s="0">
-        <v>330.219</v>
-      </c>
-      <c r="AI339" s="0">
-        <v>1418.718</v>
-      </c>
-      <c r="AJ339" s="0">
-        <v>1343.702</v>
-      </c>
-      <c r="AK339" s="0">
-        <v>866.7436</v>
-      </c>
-      <c r="AL339" s="0">
-        <v>634.0592</v>
-      </c>
-      <c r="AM339" s="0">
-        <v>1141.839</v>
-      </c>
-      <c r="AN339" s="0">
-        <v>186.7354</v>
-      </c>
-      <c r="AO339" s="0">
-        <v>334.1509</v>
-      </c>
-      <c r="AP339" s="0">
-        <v>249.5121</v>
-      </c>
-      <c r="AQ339" s="0">
-        <v>123.2064</v>
-      </c>
-      <c r="AR339" s="0">
-        <v>115.2899</v>
-      </c>
-      <c r="AS339" s="0">
-        <v>763.6548</v>
-      </c>
-      <c r="AT339" s="0">
-        <v>825.4533</v>
-      </c>
-      <c r="AU339" s="0">
-        <v>430.867</v>
-      </c>
-      <c r="AV339" s="0">
-        <v>804.7897</v>
-      </c>
-      <c r="AW339" s="0">
-        <v>229.7256</v>
-      </c>
-      <c r="AX339" s="0">
-        <v>708.8023</v>
-      </c>
-    </row>
-    <row r="340">
-      <c r="A340" s="0" t="s">
-        <v>388</v>
-      </c>
-      <c r="B340" s="0">
-        <v>317.1556</v>
-      </c>
-      <c r="C340" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D340" s="0">
-        <v>106.474</v>
-      </c>
-      <c r="E340" s="0">
-        <v>154.2856</v>
-      </c>
-      <c r="F340" s="0">
-        <v>1172.139</v>
-      </c>
-      <c r="G340" s="0">
-        <v>347.5609</v>
-      </c>
-      <c r="H340" s="0">
-        <v>473.7214</v>
-      </c>
-      <c r="I340" s="0">
-        <v>269.404</v>
-      </c>
-      <c r="J340" s="0">
-        <v>587.5497</v>
-      </c>
-      <c r="K340" s="0">
-        <v>791.6908</v>
-      </c>
-      <c r="L340" s="0">
-        <v>444.5601</v>
-      </c>
-      <c r="M340" s="0">
-        <v>1147.91</v>
-      </c>
-      <c r="N340" s="0">
-        <v>336.7523</v>
-      </c>
-      <c r="O340" s="0">
-        <v>231.3399</v>
-      </c>
-      <c r="P340" s="0">
-        <v>239.8561</v>
-      </c>
-      <c r="Q340" s="0">
-        <v>270.8528</v>
-      </c>
-      <c r="R340" s="0">
-        <v>169.3017</v>
-      </c>
-      <c r="S340" s="0">
-        <v>325.2468</v>
-      </c>
-      <c r="T340" s="0">
-        <v>333.0557</v>
-      </c>
-      <c r="U340" s="0">
-        <v>347.9297</v>
-      </c>
-      <c r="V340" s="0">
-        <v>272.9417</v>
-      </c>
-      <c r="W340" s="0">
-        <v>117.4054</v>
-      </c>
-      <c r="X340" s="0">
-        <v>214.4867</v>
-      </c>
-      <c r="Y340" s="0">
-        <v>699.3534</v>
-      </c>
-      <c r="Z340" s="0">
-        <v>510.3635</v>
-      </c>
-      <c r="AA340" s="0">
-        <v>242.5398</v>
-      </c>
-      <c r="AB340" s="0">
-        <v>179.0883</v>
-      </c>
-      <c r="AC340" s="0">
-        <v>130.4928</v>
-      </c>
-      <c r="AD340" s="0">
-        <v>684.047</v>
-      </c>
-      <c r="AE340" s="0">
-        <v>538.8293</v>
-      </c>
-      <c r="AF340" s="0">
-        <v>402.488</v>
-      </c>
-      <c r="AG340" s="0">
-        <v>168.9326</v>
-      </c>
-      <c r="AH340" s="0">
-        <v>323.4154</v>
-      </c>
-      <c r="AI340" s="0">
-        <v>1380.209</v>
-      </c>
-      <c r="AJ340" s="0">
-        <v>1299.113</v>
-      </c>
-      <c r="AK340" s="0">
-        <v>840.8714</v>
-      </c>
-      <c r="AL340" s="0">
-        <v>628.1866</v>
-      </c>
-      <c r="AM340" s="0">
-        <v>1132.558</v>
-      </c>
-      <c r="AN340" s="0">
-        <v>180.9452</v>
-      </c>
-      <c r="AO340" s="0">
-        <v>326.2636</v>
-      </c>
-      <c r="AP340" s="0">
-        <v>247.238</v>
-      </c>
-      <c r="AQ340" s="0">
-        <v>122.4609</v>
-      </c>
-      <c r="AR340" s="0">
-        <v>112.1588</v>
-      </c>
-      <c r="AS340" s="0">
-        <v>747.5975</v>
-      </c>
-      <c r="AT340" s="0">
-        <v>812.7184</v>
-      </c>
-      <c r="AU340" s="0">
-        <v>415.3195</v>
-      </c>
-      <c r="AV340" s="0">
-        <v>799.0353</v>
-      </c>
-      <c r="AW340" s="0">
-        <v>225.0562</v>
-      </c>
-      <c r="AX340" s="0">
-        <v>699.3776</v>
-      </c>
-    </row>
-    <row r="341">
-      <c r="A341" s="0" t="s">
-        <v>389</v>
-      </c>
-      <c r="B341" s="0">
-        <v>316.5096</v>
-      </c>
-      <c r="C341" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D341" s="0">
-        <v>105.6162</v>
-      </c>
-      <c r="E341" s="0">
-        <v>155.4768</v>
-      </c>
-      <c r="F341" s="0">
-        <v>1172.893</v>
-      </c>
-      <c r="G341" s="0">
-        <v>347.1196</v>
-      </c>
-      <c r="H341" s="0">
-        <v>473.2432</v>
-      </c>
-      <c r="I341" s="0">
-        <v>265.3924</v>
-      </c>
-      <c r="J341" s="0">
-        <v>588.7982</v>
-      </c>
-      <c r="K341" s="0">
-        <v>789.9759</v>
-      </c>
-      <c r="L341" s="0">
-        <v>444.9677</v>
-      </c>
-      <c r="M341" s="0">
-        <v>1126.741</v>
-      </c>
-      <c r="N341" s="0">
-        <v>335.3012</v>
-      </c>
-      <c r="O341" s="0">
-        <v>228.628</v>
-      </c>
-      <c r="P341" s="0">
-        <v>239.2081</v>
-      </c>
-      <c r="Q341" s="0">
-        <v>271.8354</v>
-      </c>
-      <c r="R341" s="0">
-        <v>169.389</v>
-      </c>
-      <c r="S341" s="0">
-        <v>324.7847</v>
-      </c>
-      <c r="T341" s="0">
-        <v>330.4554</v>
-      </c>
-      <c r="U341" s="0">
-        <v>345.3626</v>
-      </c>
-      <c r="V341" s="0">
-        <v>273.3662</v>
-      </c>
-      <c r="W341" s="0">
-        <v>115.9615</v>
-      </c>
-      <c r="X341" s="0">
-        <v>213.4922</v>
-      </c>
-      <c r="Y341" s="0">
-        <v>700.7486</v>
-      </c>
-      <c r="Z341" s="0">
-        <v>512.9776</v>
-      </c>
-      <c r="AA341" s="0">
-        <v>239.095</v>
-      </c>
-      <c r="AB341" s="0">
-        <v>179.3607</v>
-      </c>
-      <c r="AC341" s="0">
-        <v>129.8022</v>
-      </c>
-      <c r="AD341" s="0">
-        <v>682.6346</v>
-      </c>
-      <c r="AE341" s="0">
-        <v>536.3449</v>
-      </c>
-      <c r="AF341" s="0">
-        <v>402.0001</v>
-      </c>
-      <c r="AG341" s="0">
-        <v>168.24</v>
-      </c>
-      <c r="AH341" s="0">
-        <v>319.2784</v>
-      </c>
-      <c r="AI341" s="0">
-        <v>1371.521</v>
-      </c>
-      <c r="AJ341" s="0">
-        <v>1286.741</v>
-      </c>
-      <c r="AK341" s="0">
-        <v>840.4871</v>
-      </c>
-      <c r="AL341" s="0">
-        <v>629.5453</v>
-      </c>
-      <c r="AM341" s="0">
-        <v>1125.921</v>
-      </c>
-      <c r="AN341" s="0">
-        <v>179.2415</v>
-      </c>
-      <c r="AO341" s="0">
-        <v>330.1658</v>
-      </c>
-      <c r="AP341" s="0">
-        <v>247.479</v>
-      </c>
-      <c r="AQ341" s="0">
-        <v>123.0093</v>
-      </c>
-      <c r="AR341" s="0">
-        <v>109.9876</v>
-      </c>
-      <c r="AS341" s="0">
-        <v>740.7641</v>
-      </c>
-      <c r="AT341" s="0">
-        <v>805.2388</v>
-      </c>
-      <c r="AU341" s="0">
-        <v>413.4615</v>
-      </c>
-      <c r="AV341" s="0">
-        <v>872.418</v>
-      </c>
-      <c r="AW341" s="0">
-        <v>225.0979</v>
-      </c>
-      <c r="AX341" s="0">
-        <v>696.1613</v>
-      </c>
-    </row>
-    <row r="342">
-      <c r="A342" s="0" t="s">
-        <v>390</v>
-      </c>
-      <c r="B342" s="0">
-        <v>319.2406</v>
-      </c>
-      <c r="C342" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D342" s="0">
-        <v>104.9807</v>
-      </c>
-      <c r="E342" s="0">
-        <v>156.3647</v>
-      </c>
-      <c r="F342" s="0">
-        <v>1176.307</v>
-      </c>
-      <c r="G342" s="0">
-        <v>347.7349</v>
-      </c>
-      <c r="H342" s="0">
-        <v>472.1225</v>
-      </c>
-      <c r="I342" s="0">
-        <v>270.0724</v>
-      </c>
-      <c r="J342" s="0">
-        <v>593.402</v>
-      </c>
-      <c r="K342" s="0">
-        <v>790.662</v>
-      </c>
-      <c r="L342" s="0">
-        <v>445.5193</v>
-      </c>
-      <c r="M342" s="0">
-        <v>1106.356</v>
-      </c>
-      <c r="N342" s="0">
-        <v>336.8332</v>
-      </c>
-      <c r="O342" s="0">
-        <v>233.9688</v>
-      </c>
-      <c r="P342" s="0">
-        <v>237.8577</v>
-      </c>
-      <c r="Q342" s="0">
-        <v>275.4213</v>
-      </c>
-      <c r="R342" s="0">
-        <v>169.9405</v>
-      </c>
-      <c r="S342" s="0">
-        <v>324.6277</v>
-      </c>
-      <c r="T342" s="0">
-        <v>331.4055</v>
-      </c>
-      <c r="U342" s="0">
-        <v>347.6244</v>
-      </c>
-      <c r="V342" s="0">
-        <v>273.8514</v>
-      </c>
-      <c r="W342" s="0">
-        <v>115.1365</v>
-      </c>
-      <c r="X342" s="0">
-        <v>213.2908</v>
-      </c>
-      <c r="Y342" s="0">
-        <v>703.0647</v>
-      </c>
-      <c r="Z342" s="0">
-        <v>512.8454</v>
-      </c>
-      <c r="AA342" s="0">
-        <v>239.9254</v>
-      </c>
-      <c r="AB342" s="0">
-        <v>179.584</v>
-      </c>
-      <c r="AC342" s="0">
-        <v>129.5087</v>
-      </c>
-      <c r="AD342" s="0">
-        <v>685.3136</v>
-      </c>
-      <c r="AE342" s="0">
-        <v>534.6628</v>
-      </c>
-      <c r="AF342" s="0">
-        <v>401.0148</v>
-      </c>
-      <c r="AG342" s="0">
-        <v>171.8413</v>
-      </c>
-      <c r="AH342" s="0">
-        <v>322.5105</v>
-      </c>
-      <c r="AI342" s="0">
-        <v>1367.42</v>
-      </c>
-      <c r="AJ342" s="0">
-        <v>1291.487</v>
-      </c>
-      <c r="AK342" s="0">
-        <v>842.1956</v>
-      </c>
-      <c r="AL342" s="0">
-        <v>629.9837</v>
-      </c>
-      <c r="AM342" s="0">
-        <v>1103.407</v>
-      </c>
-      <c r="AN342" s="0">
-        <v>179.7991</v>
-      </c>
-      <c r="AO342" s="0">
-        <v>328.7961</v>
-      </c>
-      <c r="AP342" s="0">
-        <v>248.0611</v>
-      </c>
-      <c r="AQ342" s="0">
-        <v>123.4</v>
-      </c>
-      <c r="AR342" s="0">
-        <v>111.5067</v>
-      </c>
-      <c r="AS342" s="0">
-        <v>739.2798</v>
-      </c>
-      <c r="AT342" s="0">
-        <v>805.6719</v>
-      </c>
-      <c r="AU342" s="0">
-        <v>410.4734</v>
-      </c>
-      <c r="AV342" s="0">
-        <v>888.7829</v>
-      </c>
-      <c r="AW342" s="0">
-        <v>225.2094</v>
-      </c>
-      <c r="AX342" s="0">
-        <v>698.2428</v>
-      </c>
-    </row>
-    <row r="343">
-      <c r="A343" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="B343" s="0">
-        <v>304.3766</v>
-      </c>
-      <c r="C343" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D343" s="0">
-        <v>102.8353</v>
-      </c>
-      <c r="E343" s="0">
-        <v>156.2425</v>
-      </c>
-      <c r="F343" s="0">
-        <v>1151.271</v>
-      </c>
-      <c r="G343" s="0">
-        <v>342.3955</v>
-      </c>
-      <c r="H343" s="0">
-        <v>470.4853</v>
-      </c>
-      <c r="I343" s="0">
-        <v>261.8777</v>
-      </c>
-      <c r="J343" s="0">
-        <v>581.5876</v>
-      </c>
-      <c r="K343" s="0">
-        <v>772.6012</v>
-      </c>
-      <c r="L343" s="0">
-        <v>434.0406</v>
-      </c>
-      <c r="M343" s="0">
-        <v>1057.787</v>
-      </c>
-      <c r="N343" s="0">
-        <v>327.6821</v>
-      </c>
-      <c r="O343" s="0">
-        <v>226.9164</v>
-      </c>
-      <c r="P343" s="0">
-        <v>234.1939</v>
-      </c>
-      <c r="Q343" s="0">
-        <v>273.5428</v>
-      </c>
-      <c r="R343" s="0">
-        <v>168.011</v>
-      </c>
-      <c r="S343" s="0">
-        <v>321.3049</v>
-      </c>
-      <c r="T343" s="0">
-        <v>324.612</v>
-      </c>
-      <c r="U343" s="0">
-        <v>341.2124</v>
-      </c>
-      <c r="V343" s="0">
-        <v>266.0767</v>
-      </c>
-      <c r="W343" s="0">
-        <v>111.0313</v>
-      </c>
-      <c r="X343" s="0">
-        <v>210.1886</v>
-      </c>
-      <c r="Y343" s="0">
-        <v>682.735</v>
-      </c>
-      <c r="Z343" s="0">
-        <v>484.7353</v>
-      </c>
-      <c r="AA343" s="0">
-        <v>235.36</v>
-      </c>
-      <c r="AB343" s="0">
-        <v>178.5374</v>
-      </c>
-      <c r="AC343" s="0">
-        <v>126.9984</v>
-      </c>
-      <c r="AD343" s="0">
-        <v>667.8707</v>
-      </c>
-      <c r="AE343" s="0">
-        <v>518.4341</v>
-      </c>
-      <c r="AF343" s="0">
-        <v>395.7309</v>
-      </c>
-      <c r="AG343" s="0">
-        <v>166.2936</v>
-      </c>
-      <c r="AH343" s="0">
-        <v>317.5273</v>
-      </c>
-      <c r="AI343" s="0">
-        <v>1347.899</v>
-      </c>
-      <c r="AJ343" s="0">
-        <v>1267.883</v>
-      </c>
-      <c r="AK343" s="0">
-        <v>829.6157</v>
-      </c>
-      <c r="AL343" s="0">
-        <v>624.674</v>
-      </c>
-      <c r="AM343" s="0">
-        <v>1093.788</v>
-      </c>
-      <c r="AN343" s="0">
-        <v>171.2757</v>
-      </c>
-      <c r="AO343" s="0">
-        <v>322.1214</v>
-      </c>
-      <c r="AP343" s="0">
-        <v>246.2144</v>
-      </c>
-      <c r="AQ343" s="0">
-        <v>121.2085</v>
-      </c>
-      <c r="AR343" s="0">
-        <v>108.2398</v>
-      </c>
-      <c r="AS343" s="0">
-        <v>706.2339</v>
-      </c>
-      <c r="AT343" s="0">
-        <v>787.6937</v>
-      </c>
-      <c r="AU343" s="0">
-        <v>399.2522</v>
-      </c>
-      <c r="AV343" s="0">
-        <v>825.0752</v>
-      </c>
-      <c r="AW343" s="0">
-        <v>224.2309</v>
-      </c>
-      <c r="AX343" s="0">
-        <v>687.1114</v>
-      </c>
-    </row>
-    <row r="344">
-      <c r="A344" s="0" t="s">
-        <v>392</v>
-      </c>
-      <c r="B344" s="0">
-        <v>295.4034</v>
-      </c>
-      <c r="C344" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D344" s="0">
-        <v>103.5552</v>
-      </c>
-      <c r="E344" s="0">
-        <v>158.4249</v>
-      </c>
-      <c r="F344" s="0">
-        <v>1112.535</v>
-      </c>
-      <c r="G344" s="0">
-        <v>343.6362</v>
-      </c>
-      <c r="H344" s="0">
-        <v>472.9505</v>
-      </c>
-      <c r="I344" s="0">
-        <v>257.4562</v>
-      </c>
-      <c r="J344" s="0">
-        <v>582.2828</v>
-      </c>
-      <c r="K344" s="0">
-        <v>766.3687</v>
-      </c>
-      <c r="L344" s="0">
-        <v>431.1082</v>
-      </c>
-      <c r="M344" s="0">
-        <v>1054.746</v>
-      </c>
-      <c r="N344" s="0">
-        <v>318.6516</v>
-      </c>
-      <c r="O344" s="0">
-        <v>219.5798</v>
-      </c>
-      <c r="P344" s="0">
-        <v>235.0273</v>
-      </c>
-      <c r="Q344" s="0">
-        <v>267.1781</v>
-      </c>
-      <c r="R344" s="0">
-        <v>168.2983</v>
-      </c>
-      <c r="S344" s="0">
-        <v>321.3477</v>
-      </c>
-      <c r="T344" s="0">
-        <v>324.7639</v>
-      </c>
-      <c r="U344" s="0">
-        <v>335.6526</v>
-      </c>
-      <c r="V344" s="0">
-        <v>265.5718</v>
-      </c>
-      <c r="W344" s="0">
-        <v>110.098</v>
-      </c>
-      <c r="X344" s="0">
-        <v>210.0107</v>
-      </c>
-      <c r="Y344" s="0">
-        <v>674.9118</v>
-      </c>
-      <c r="Z344" s="0">
-        <v>468.5415</v>
-      </c>
-      <c r="AA344" s="0">
-        <v>234.0749</v>
-      </c>
-      <c r="AB344" s="0">
-        <v>179.12</v>
-      </c>
-      <c r="AC344" s="0">
-        <v>127.1089</v>
-      </c>
-      <c r="AD344" s="0">
-        <v>661.2296</v>
-      </c>
-      <c r="AE344" s="0">
-        <v>510.008</v>
-      </c>
-      <c r="AF344" s="0">
-        <v>395.7453</v>
-      </c>
-      <c r="AG344" s="0">
-        <v>160.2235</v>
-      </c>
-      <c r="AH344" s="0">
-        <v>307.3803</v>
-      </c>
-      <c r="AI344" s="0">
-        <v>1352.008</v>
-      </c>
-      <c r="AJ344" s="0">
-        <v>1274.878</v>
-      </c>
-      <c r="AK344" s="0">
-        <v>828.6467</v>
-      </c>
-      <c r="AL344" s="0">
-        <v>626.7437</v>
-      </c>
-      <c r="AM344" s="0">
-        <v>1097.815</v>
-      </c>
-      <c r="AN344" s="0">
-        <v>165.3265</v>
-      </c>
-      <c r="AO344" s="0">
-        <v>319.0902</v>
-      </c>
-      <c r="AP344" s="0">
-        <v>247.1374</v>
-      </c>
-      <c r="AQ344" s="0">
-        <v>120.5987</v>
-      </c>
-      <c r="AR344" s="0">
-        <v>106.156</v>
-      </c>
-      <c r="AS344" s="0">
-        <v>692.2092</v>
-      </c>
-      <c r="AT344" s="0">
-        <v>776.7358</v>
-      </c>
-      <c r="AU344" s="0">
-        <v>402.4063</v>
-      </c>
-      <c r="AV344" s="0">
-        <v>802.3913</v>
-      </c>
-      <c r="AW344" s="0">
-        <v>223.7665</v>
-      </c>
-      <c r="AX344" s="0">
-        <v>679.3539</v>
-      </c>
-    </row>
-    <row r="345">
-      <c r="A345" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="B345" s="0">
-        <v>289.4506</v>
-      </c>
-      <c r="C345" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D345" s="0">
-        <v>104.9031</v>
-      </c>
-      <c r="E345" s="0">
-        <v>159.6785</v>
-      </c>
-      <c r="F345" s="0">
-        <v>1145.21</v>
-      </c>
-      <c r="G345" s="0">
-        <v>347.2763</v>
-      </c>
-      <c r="H345" s="0">
-        <v>473.9158</v>
-      </c>
-      <c r="I345" s="0">
-        <v>263.1056</v>
-      </c>
-      <c r="J345" s="0">
-        <v>597.2043</v>
-      </c>
-      <c r="K345" s="0">
-        <v>777.883</v>
-      </c>
-      <c r="L345" s="0">
-        <v>440.0701</v>
-      </c>
-      <c r="M345" s="0">
-        <v>1095.907</v>
-      </c>
-      <c r="N345" s="0">
-        <v>325.3009</v>
-      </c>
-      <c r="O345" s="0">
-        <v>217.089</v>
-      </c>
-      <c r="P345" s="0">
-        <v>237.667</v>
-      </c>
-      <c r="Q345" s="0">
-        <v>276.0531</v>
-      </c>
-      <c r="R345" s="0">
-        <v>170.4729</v>
-      </c>
-      <c r="S345" s="0">
-        <v>324.4215</v>
-      </c>
-      <c r="T345" s="0">
-        <v>330.0518</v>
-      </c>
-      <c r="U345" s="0">
-        <v>342.3372</v>
-      </c>
-      <c r="V345" s="0">
-        <v>270.5492</v>
-      </c>
-      <c r="W345" s="0">
-        <v>113.9917</v>
-      </c>
-      <c r="X345" s="0">
-        <v>215.4699</v>
-      </c>
-      <c r="Y345" s="0">
-        <v>687.5871</v>
-      </c>
-      <c r="Z345" s="0">
-        <v>476.0433</v>
-      </c>
-      <c r="AA345" s="0">
-        <v>237.0815</v>
-      </c>
-      <c r="AB345" s="0">
-        <v>180.4354</v>
-      </c>
-      <c r="AC345" s="0">
-        <v>129.4905</v>
-      </c>
-      <c r="AD345" s="0">
-        <v>681.1857</v>
-      </c>
-      <c r="AE345" s="0">
-        <v>520.3814</v>
-      </c>
-      <c r="AF345" s="0">
-        <v>397.4014</v>
-      </c>
-      <c r="AG345" s="0">
-        <v>163.6685</v>
-      </c>
-      <c r="AH345" s="0">
-        <v>312.4186</v>
-      </c>
-      <c r="AI345" s="0">
-        <v>1377.513</v>
-      </c>
-      <c r="AJ345" s="0">
-        <v>1301.155</v>
-      </c>
-      <c r="AK345" s="0">
-        <v>838.6196</v>
-      </c>
-      <c r="AL345" s="0">
-        <v>629.5316</v>
-      </c>
-      <c r="AM345" s="0">
-        <v>1124.895</v>
-      </c>
-      <c r="AN345" s="0">
-        <v>170.4031</v>
-      </c>
-      <c r="AO345" s="0">
-        <v>325.8104</v>
-      </c>
-      <c r="AP345" s="0">
-        <v>249.2765</v>
-      </c>
-      <c r="AQ345" s="0">
-        <v>120.9539</v>
-      </c>
-      <c r="AR345" s="0">
-        <v>108.2434</v>
-      </c>
-      <c r="AS345" s="0">
-        <v>694.7425</v>
-      </c>
-      <c r="AT345" s="0">
-        <v>781.2904</v>
-      </c>
-      <c r="AU345" s="0">
-        <v>414.9454</v>
-      </c>
-      <c r="AV345" s="0">
-        <v>789.7583</v>
-      </c>
-      <c r="AW345" s="0">
-        <v>224.6508</v>
-      </c>
-      <c r="AX345" s="0">
-        <v>689.465</v>
-      </c>
-    </row>
-    <row r="346">
-      <c r="A346" s="0" t="s">
-        <v>394</v>
-      </c>
-      <c r="B346" s="0">
-        <v>273.4745</v>
-      </c>
-      <c r="C346" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D346" s="0">
-        <v>103.737</v>
-      </c>
-      <c r="E346" s="0">
-        <v>160.7962</v>
-      </c>
-      <c r="F346" s="0">
-        <v>1140.304</v>
-      </c>
-      <c r="G346" s="0">
-        <v>347.3687</v>
-      </c>
-      <c r="H346" s="0">
-        <v>476.6132</v>
-      </c>
-      <c r="I346" s="0">
-        <v>255.4265</v>
-      </c>
-      <c r="J346" s="0">
-        <v>597.4313</v>
-      </c>
-      <c r="K346" s="0">
-        <v>771.5376</v>
-      </c>
-      <c r="L346" s="0">
-        <v>439.2176</v>
-      </c>
-      <c r="M346" s="0">
-        <v>1089.371</v>
-      </c>
-      <c r="N346" s="0">
-        <v>322.9587</v>
-      </c>
-      <c r="O346" s="0">
-        <v>218.9657</v>
-      </c>
-      <c r="P346" s="0">
-        <v>237.6504</v>
-      </c>
-      <c r="Q346" s="0">
-        <v>271.6772</v>
-      </c>
-      <c r="R346" s="0">
-        <v>170.7391</v>
-      </c>
-      <c r="S346" s="0">
-        <v>325.4629</v>
-      </c>
-      <c r="T346" s="0">
-        <v>332.7205</v>
-      </c>
-      <c r="U346" s="0">
-        <v>340.6935</v>
-      </c>
-      <c r="V346" s="0">
-        <v>272.6119</v>
-      </c>
-      <c r="W346" s="0">
-        <v>112.3907</v>
-      </c>
-      <c r="X346" s="0">
-        <v>215.994</v>
-      </c>
-      <c r="Y346" s="0">
-        <v>679.6042</v>
-      </c>
-      <c r="Z346" s="0">
-        <v>474.078</v>
-      </c>
-      <c r="AA346" s="0">
-        <v>239.0045</v>
-      </c>
-      <c r="AB346" s="0">
-        <v>181.0331</v>
-      </c>
-      <c r="AC346" s="0">
-        <v>129.7162</v>
-      </c>
-      <c r="AD346" s="0">
-        <v>676.5443</v>
-      </c>
-      <c r="AE346" s="0">
-        <v>518.6299</v>
-      </c>
-      <c r="AF346" s="0">
-        <v>402.6101</v>
-      </c>
-      <c r="AG346" s="0">
-        <v>160.8577</v>
-      </c>
-      <c r="AH346" s="0">
-        <v>319.1073</v>
-      </c>
-      <c r="AI346" s="0">
-        <v>1378.382</v>
-      </c>
-      <c r="AJ346" s="0">
-        <v>1305.067</v>
-      </c>
-      <c r="AK346" s="0">
-        <v>846.8698</v>
-      </c>
-      <c r="AL346" s="0">
-        <v>631.7784</v>
-      </c>
-      <c r="AM346" s="0">
-        <v>1100.332</v>
-      </c>
-      <c r="AN346" s="0">
-        <v>167.393</v>
-      </c>
-      <c r="AO346" s="0">
-        <v>319.7159</v>
-      </c>
-      <c r="AP346" s="0">
-        <v>249.6775</v>
-      </c>
-      <c r="AQ346" s="0">
-        <v>120.8046</v>
-      </c>
-      <c r="AR346" s="0">
-        <v>107.5403</v>
-      </c>
-      <c r="AS346" s="0">
-        <v>653.225</v>
-      </c>
-      <c r="AT346" s="0">
-        <v>782.9654</v>
-      </c>
-      <c r="AU346" s="0">
-        <v>416.2283</v>
-      </c>
-      <c r="AV346" s="0">
-        <v>749.527</v>
-      </c>
-      <c r="AW346" s="0">
-        <v>227.7138</v>
-      </c>
-      <c r="AX346" s="0">
-        <v>683.1953</v>
-      </c>
-    </row>
-    <row r="347">
-      <c r="A347" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="B347" s="0">
-        <v>273.5535</v>
-      </c>
-      <c r="C347" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D347" s="0">
-        <v>104.5584</v>
-      </c>
-      <c r="E347" s="0">
-        <v>158.9768</v>
-      </c>
-      <c r="F347" s="0">
-        <v>1125.41</v>
-      </c>
-      <c r="G347" s="0">
-        <v>347.0084</v>
-      </c>
-      <c r="H347" s="0">
-        <v>475.7691</v>
-      </c>
-      <c r="I347" s="0">
-        <v>258.3897</v>
-      </c>
-      <c r="J347" s="0">
-        <v>597.0038</v>
-      </c>
-      <c r="K347" s="0">
-        <v>769.0236</v>
-      </c>
-      <c r="L347" s="0">
-        <v>438.888</v>
-      </c>
-      <c r="M347" s="0">
-        <v>1088.272</v>
-      </c>
-      <c r="N347" s="0">
-        <v>321.1274</v>
-      </c>
-      <c r="O347" s="0">
-        <v>225.6268</v>
-      </c>
-      <c r="P347" s="0">
-        <v>238.8546</v>
-      </c>
-      <c r="Q347" s="0">
-        <v>273.3616</v>
-      </c>
-      <c r="R347" s="0">
-        <v>171.5384</v>
-      </c>
-      <c r="S347" s="0">
-        <v>326.8319</v>
-      </c>
-      <c r="T347" s="0">
-        <v>328.6086</v>
-      </c>
-      <c r="U347" s="0">
-        <v>345.215</v>
-      </c>
-      <c r="V347" s="0">
-        <v>272.8672</v>
-      </c>
-      <c r="W347" s="0">
-        <v>112.5892</v>
-      </c>
-      <c r="X347" s="0">
-        <v>217.5385</v>
-      </c>
-      <c r="Y347" s="0">
-        <v>676.1999</v>
-      </c>
-      <c r="Z347" s="0">
-        <v>456.053</v>
-      </c>
-      <c r="AA347" s="0">
-        <v>234.7771</v>
-      </c>
-      <c r="AB347" s="0">
-        <v>181.383</v>
-      </c>
-      <c r="AC347" s="0">
-        <v>130.1521</v>
-      </c>
-      <c r="AD347" s="0">
-        <v>678.7582</v>
-      </c>
-      <c r="AE347" s="0">
-        <v>514.1695</v>
-      </c>
-      <c r="AF347" s="0">
-        <v>402.0408</v>
-      </c>
-      <c r="AG347" s="0">
-        <v>161.8867</v>
-      </c>
-      <c r="AH347" s="0">
-        <v>321.407</v>
-      </c>
-      <c r="AI347" s="0">
-        <v>1382.02</v>
-      </c>
-      <c r="AJ347" s="0">
-        <v>1308.004</v>
-      </c>
-      <c r="AK347" s="0">
-        <v>845.8066</v>
-      </c>
-      <c r="AL347" s="0">
-        <v>634.5387</v>
-      </c>
-      <c r="AM347" s="0">
-        <v>1095.405</v>
-      </c>
-      <c r="AN347" s="0">
-        <v>169.3536</v>
-      </c>
-      <c r="AO347" s="0">
-        <v>317.3369</v>
-      </c>
-      <c r="AP347" s="0">
-        <v>250.4059</v>
-      </c>
-      <c r="AQ347" s="0">
-        <v>118.9419</v>
-      </c>
-      <c r="AR347" s="0">
-        <v>104.7249</v>
-      </c>
-      <c r="AS347" s="0">
-        <v>665.2134</v>
-      </c>
-      <c r="AT347" s="0">
-        <v>782.2969</v>
-      </c>
-      <c r="AU347" s="0">
-        <v>414.6461</v>
-      </c>
-      <c r="AV347" s="0">
-        <v>683.0927</v>
-      </c>
-      <c r="AW347" s="0">
-        <v>228.9123</v>
-      </c>
-      <c r="AX347" s="0">
-        <v>672.5812</v>
-      </c>
-    </row>
-    <row r="348">
-      <c r="A348" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="B348" s="0">
-        <v>274.6518</v>
-      </c>
-      <c r="C348" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D348" s="0">
-        <v>106.0127</v>
-      </c>
-      <c r="E348" s="0">
-        <v>159.985</v>
-      </c>
-      <c r="F348" s="0">
-        <v>1161.322</v>
-      </c>
-      <c r="G348" s="0">
-        <v>344.5172</v>
-      </c>
-      <c r="H348" s="0">
-        <v>474.6042</v>
-      </c>
-      <c r="I348" s="0">
-        <v>259.7281</v>
-      </c>
-      <c r="J348" s="0">
-        <v>588.8986</v>
-      </c>
-      <c r="K348" s="0">
-        <v>769.1656</v>
-      </c>
-      <c r="L348" s="0">
-        <v>437.8333</v>
-      </c>
-      <c r="M348" s="0">
-        <v>1099.859</v>
-      </c>
-      <c r="N348" s="0">
-        <v>323.0741</v>
-      </c>
-      <c r="O348" s="0">
-        <v>224.5016</v>
-      </c>
-      <c r="P348" s="0">
-        <v>239.8781</v>
-      </c>
-      <c r="Q348" s="0">
-        <v>270.0891</v>
-      </c>
-      <c r="R348" s="0">
-        <v>171.4433</v>
-      </c>
-      <c r="S348" s="0">
-        <v>325.6739</v>
-      </c>
-      <c r="T348" s="0">
-        <v>324.6473</v>
-      </c>
-      <c r="U348" s="0">
-        <v>348.7262</v>
-      </c>
-      <c r="V348" s="0">
-        <v>276.1298</v>
-      </c>
-      <c r="W348" s="0">
-        <v>113.4231</v>
-      </c>
-      <c r="X348" s="0">
-        <v>217.0824</v>
-      </c>
-      <c r="Y348" s="0">
-        <v>675.2284</v>
-      </c>
-      <c r="Z348" s="0">
-        <v>470.7581</v>
-      </c>
-      <c r="AA348" s="0">
-        <v>231.4803</v>
-      </c>
-      <c r="AB348" s="0">
-        <v>181.2588</v>
-      </c>
-      <c r="AC348" s="0">
-        <v>128.9041</v>
-      </c>
-      <c r="AD348" s="0">
-        <v>672.8229</v>
-      </c>
-      <c r="AE348" s="0">
-        <v>520.7319</v>
-      </c>
-      <c r="AF348" s="0">
-        <v>401.1525</v>
-      </c>
-      <c r="AG348" s="0">
-        <v>161.9701</v>
-      </c>
-      <c r="AH348" s="0">
-        <v>326.102</v>
-      </c>
-      <c r="AI348" s="0">
-        <v>1363.597</v>
-      </c>
-      <c r="AJ348" s="0">
-        <v>1287.016</v>
-      </c>
-      <c r="AK348" s="0">
-        <v>832.965</v>
-      </c>
-      <c r="AL348" s="0">
-        <v>631.3113</v>
-      </c>
-      <c r="AM348" s="0">
-        <v>1100.26</v>
-      </c>
-      <c r="AN348" s="0">
-        <v>167.486</v>
-      </c>
-      <c r="AO348" s="0">
-        <v>311.1491</v>
-      </c>
-      <c r="AP348" s="0">
-        <v>250.7018</v>
-      </c>
-      <c r="AQ348" s="0">
-        <v>117.5024</v>
-      </c>
-      <c r="AR348" s="0">
-        <v>104.8659</v>
-      </c>
-      <c r="AS348" s="0">
-        <v>683.4281</v>
-      </c>
-      <c r="AT348" s="0">
-        <v>783.2204</v>
-      </c>
-      <c r="AU348" s="0">
-        <v>407.488</v>
-      </c>
-      <c r="AV348" s="0">
-        <v>716.8712</v>
-      </c>
-      <c r="AW348" s="0">
-        <v>227.8313</v>
-      </c>
-      <c r="AX348" s="0">
-        <v>674.6974</v>
-      </c>
-    </row>
-    <row r="349">
-      <c r="A349" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="B349" s="0">
-        <v>277.8009</v>
-      </c>
-      <c r="C349" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D349" s="0">
-        <v>104.3122</v>
-      </c>
-      <c r="E349" s="0">
-        <v>156.4461</v>
-      </c>
-      <c r="F349" s="0">
-        <v>1172.978</v>
-      </c>
-      <c r="G349" s="0">
-        <v>341.22</v>
-      </c>
-      <c r="H349" s="0">
-        <v>475.7919</v>
-      </c>
-      <c r="I349" s="0">
-        <v>253.1214</v>
-      </c>
-      <c r="J349" s="0">
-        <v>579.276</v>
-      </c>
-      <c r="K349" s="0">
-        <v>760.51</v>
-      </c>
-      <c r="L349" s="0">
-        <v>434.3516</v>
-      </c>
-      <c r="M349" s="0">
-        <v>1075.441</v>
-      </c>
-      <c r="N349" s="0">
-        <v>318.5509</v>
-      </c>
-      <c r="O349" s="0">
-        <v>218.7596</v>
-      </c>
-      <c r="P349" s="0">
-        <v>240.8866</v>
-      </c>
-      <c r="Q349" s="0">
-        <v>261.1465</v>
-      </c>
-      <c r="R349" s="0">
-        <v>171.2886</v>
-      </c>
-      <c r="S349" s="0">
-        <v>324.7999</v>
-      </c>
-      <c r="T349" s="0">
-        <v>322.0417</v>
-      </c>
-      <c r="U349" s="0">
-        <v>344.7586</v>
-      </c>
-      <c r="V349" s="0">
-        <v>273.0611</v>
-      </c>
-      <c r="W349" s="0">
-        <v>111.3924</v>
-      </c>
-      <c r="X349" s="0">
-        <v>212.7477</v>
-      </c>
-      <c r="Y349" s="0">
-        <v>662.2728</v>
-      </c>
-      <c r="Z349" s="0">
-        <v>463.9563</v>
-      </c>
-      <c r="AA349" s="0">
-        <v>222.5707</v>
-      </c>
-      <c r="AB349" s="0">
-        <v>181.5749</v>
-      </c>
-      <c r="AC349" s="0">
-        <v>128.2081</v>
-      </c>
-      <c r="AD349" s="0">
-        <v>644.2001</v>
-      </c>
-      <c r="AE349" s="0">
-        <v>511.859</v>
-      </c>
-      <c r="AF349" s="0">
-        <v>399.677</v>
-      </c>
-      <c r="AG349" s="0">
-        <v>156.0159</v>
-      </c>
-      <c r="AH349" s="0">
-        <v>325.6959</v>
-      </c>
-      <c r="AI349" s="0">
-        <v>1348.201</v>
-      </c>
-      <c r="AJ349" s="0">
-        <v>1277.249</v>
-      </c>
-      <c r="AK349" s="0">
-        <v>836.217</v>
-      </c>
-      <c r="AL349" s="0">
-        <v>633.0597</v>
-      </c>
-      <c r="AM349" s="0">
-        <v>1095.486</v>
-      </c>
-      <c r="AN349" s="0">
-        <v>162.4854</v>
-      </c>
-      <c r="AO349" s="0">
-        <v>313.04</v>
-      </c>
-      <c r="AP349" s="0">
-        <v>250.3912</v>
-      </c>
-      <c r="AQ349" s="0">
-        <v>117.2736</v>
-      </c>
-      <c r="AR349" s="0">
-        <v>103.0319</v>
-      </c>
-      <c r="AS349" s="0">
-        <v>691.1807</v>
-      </c>
-      <c r="AT349" s="0">
-        <v>764.0864</v>
-      </c>
-      <c r="AU349" s="0">
-        <v>398.1173</v>
-      </c>
-      <c r="AV349" s="0">
-        <v>676.6566</v>
-      </c>
-      <c r="AW349" s="0">
-        <v>228.1628</v>
-      </c>
-      <c r="AX349" s="0">
-        <v>668.8738</v>
-      </c>
-    </row>
-    <row r="350">
-      <c r="A350" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="B350" s="0">
-        <v>265.0321</v>
-      </c>
-      <c r="C350" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D350" s="0">
-        <v>104.3305</v>
-      </c>
-      <c r="E350" s="0">
-        <v>157.6127</v>
-      </c>
-      <c r="F350" s="0">
-        <v>1195.156</v>
-      </c>
-      <c r="G350" s="0">
-        <v>347.4266</v>
-      </c>
-      <c r="H350" s="0">
-        <v>481.4928</v>
-      </c>
-      <c r="I350" s="0">
-        <v>253.9243</v>
-      </c>
-      <c r="J350" s="0">
-        <v>591.1074</v>
-      </c>
-      <c r="K350" s="0">
-        <v>768.8764</v>
-      </c>
-      <c r="L350" s="0">
-        <v>438.5877</v>
-      </c>
-      <c r="M350" s="0">
-        <v>1086.9</v>
-      </c>
-      <c r="N350" s="0">
-        <v>315.9252</v>
-      </c>
-      <c r="O350" s="0">
-        <v>220.6414</v>
-      </c>
-      <c r="P350" s="0">
-        <v>240.5509</v>
-      </c>
-      <c r="Q350" s="0">
-        <v>259.292</v>
-      </c>
-      <c r="R350" s="0">
-        <v>172.0175</v>
-      </c>
-      <c r="S350" s="0">
-        <v>328.2286</v>
-      </c>
-      <c r="T350" s="0">
-        <v>329.562</v>
-      </c>
-      <c r="U350" s="0">
-        <v>344.7753</v>
-      </c>
-      <c r="V350" s="0">
-        <v>273.802</v>
-      </c>
-      <c r="W350" s="0">
-        <v>112.5688</v>
-      </c>
-      <c r="X350" s="0">
-        <v>215.34</v>
-      </c>
-      <c r="Y350" s="0">
-        <v>668.4373</v>
-      </c>
-      <c r="Z350" s="0">
-        <v>465.0663</v>
-      </c>
-      <c r="AA350" s="0">
-        <v>229.0636</v>
-      </c>
-      <c r="AB350" s="0">
-        <v>182.1959</v>
-      </c>
-      <c r="AC350" s="0">
-        <v>129.7549</v>
-      </c>
-      <c r="AD350" s="0">
-        <v>656.1811</v>
-      </c>
-      <c r="AE350" s="0">
-        <v>507.5508</v>
-      </c>
-      <c r="AF350" s="0">
-        <v>404.3169</v>
-      </c>
-      <c r="AG350" s="0">
-        <v>154.8329</v>
-      </c>
-      <c r="AH350" s="0">
-        <v>326.4646</v>
-      </c>
-      <c r="AI350" s="0">
-        <v>1379.075</v>
-      </c>
-      <c r="AJ350" s="0">
-        <v>1311.454</v>
-      </c>
-      <c r="AK350" s="0">
-        <v>855.2423</v>
-      </c>
-      <c r="AL350" s="0">
-        <v>638.8117</v>
-      </c>
-      <c r="AM350" s="0">
-        <v>1112.814</v>
-      </c>
-      <c r="AN350" s="0">
-        <v>165.2663</v>
-      </c>
-      <c r="AO350" s="0">
-        <v>320.7049</v>
-      </c>
-      <c r="AP350" s="0">
-        <v>251.4943</v>
-      </c>
-      <c r="AQ350" s="0">
-        <v>117.5224</v>
-      </c>
-      <c r="AR350" s="0">
-        <v>103.4164</v>
-      </c>
-      <c r="AS350" s="0">
-        <v>709.5685</v>
-      </c>
-      <c r="AT350" s="0">
-        <v>749.5307</v>
-      </c>
-      <c r="AU350" s="0">
-        <v>410.5984</v>
-      </c>
-      <c r="AV350" s="0">
-        <v>657.1725</v>
-      </c>
-      <c r="AW350" s="0">
-        <v>229.489</v>
-      </c>
-      <c r="AX350" s="0">
-        <v>679.946</v>
-      </c>
-    </row>
-    <row r="351">
-      <c r="A351" s="0" t="s">
-        <v>399</v>
-      </c>
-      <c r="B351" s="0">
-        <v>281.3676</v>
-      </c>
-      <c r="C351" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D351" s="0">
-        <v>106.2552</v>
-      </c>
-      <c r="E351" s="0">
-        <v>155.5494</v>
-      </c>
-      <c r="F351" s="0">
-        <v>1226.134</v>
-      </c>
-      <c r="G351" s="0">
-        <v>355.0703</v>
-      </c>
-      <c r="H351" s="0">
-        <v>486.9091</v>
-      </c>
-      <c r="I351" s="0">
-        <v>262.0467</v>
-      </c>
-      <c r="J351" s="0">
-        <v>604.5752</v>
-      </c>
-      <c r="K351" s="0">
-        <v>788.8574</v>
-      </c>
-      <c r="L351" s="0">
-        <v>449.961</v>
-      </c>
-      <c r="M351" s="0">
-        <v>1129.528</v>
-      </c>
-      <c r="N351" s="0">
-        <v>322.4153</v>
-      </c>
-      <c r="O351" s="0">
-        <v>229.1856</v>
-      </c>
-      <c r="P351" s="0">
-        <v>242.6882</v>
-      </c>
-      <c r="Q351" s="0">
-        <v>265.8164</v>
-      </c>
-      <c r="R351" s="0">
-        <v>174.5432</v>
-      </c>
-      <c r="S351" s="0">
-        <v>332.1031</v>
-      </c>
-      <c r="T351" s="0">
-        <v>338.6257</v>
-      </c>
-      <c r="U351" s="0">
-        <v>351.6366</v>
-      </c>
-      <c r="V351" s="0">
-        <v>277.6982</v>
-      </c>
-      <c r="W351" s="0">
-        <v>114.9488</v>
-      </c>
-      <c r="X351" s="0">
-        <v>221.591</v>
-      </c>
-      <c r="Y351" s="0">
-        <v>691.3976</v>
-      </c>
-      <c r="Z351" s="0">
-        <v>464.7759</v>
-      </c>
-      <c r="AA351" s="0">
-        <v>236.1984</v>
-      </c>
-      <c r="AB351" s="0">
-        <v>183.1669</v>
-      </c>
-      <c r="AC351" s="0">
-        <v>131.986</v>
-      </c>
-      <c r="AD351" s="0">
-        <v>671.7763</v>
-      </c>
-      <c r="AE351" s="0">
-        <v>507.1058</v>
-      </c>
-      <c r="AF351" s="0">
-        <v>409.6268</v>
-      </c>
-      <c r="AG351" s="0">
-        <v>162.5461</v>
-      </c>
-      <c r="AH351" s="0">
-        <v>335.3737</v>
-      </c>
-      <c r="AI351" s="0">
-        <v>1404.819</v>
-      </c>
-      <c r="AJ351" s="0">
-        <v>1342.761</v>
-      </c>
-      <c r="AK351" s="0">
-        <v>873.9434</v>
-      </c>
-      <c r="AL351" s="0">
-        <v>646.8813</v>
-      </c>
-      <c r="AM351" s="0">
-        <v>1141.21</v>
-      </c>
-      <c r="AN351" s="0">
-        <v>173.6581</v>
-      </c>
-      <c r="AO351" s="0">
-        <v>329.7259</v>
-      </c>
-      <c r="AP351" s="0">
-        <v>254.0723</v>
-      </c>
-      <c r="AQ351" s="0">
-        <v>118.4518</v>
-      </c>
-      <c r="AR351" s="0">
-        <v>105.3436</v>
-      </c>
-      <c r="AS351" s="0">
-        <v>726.2437</v>
-      </c>
-      <c r="AT351" s="0">
-        <v>770.3328</v>
-      </c>
-      <c r="AU351" s="0">
-        <v>422.6088</v>
-      </c>
-      <c r="AV351" s="0">
-        <v>779.5941</v>
-      </c>
-      <c r="AW351" s="0">
-        <v>233.9708</v>
-      </c>
-      <c r="AX351" s="0">
-        <v>702.4071</v>
-      </c>
-    </row>
-    <row r="352">
-      <c r="A352" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="B352" s="0">
-        <v>287.8692</v>
-      </c>
-      <c r="C352" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D352" s="0">
-        <v>107.9953</v>
-      </c>
-      <c r="E352" s="0">
-        <v>162.6044</v>
-      </c>
-      <c r="F352" s="0">
-        <v>1246.168</v>
-      </c>
-      <c r="G352" s="0">
-        <v>361.172</v>
-      </c>
-      <c r="H352" s="0">
-        <v>491.6941</v>
-      </c>
-      <c r="I352" s="0">
-        <v>272.1868</v>
-      </c>
-      <c r="J352" s="0">
-        <v>614.1954</v>
-      </c>
-      <c r="K352" s="0">
-        <v>806.6769</v>
-      </c>
-      <c r="L352" s="0">
-        <v>459.8704</v>
-      </c>
-      <c r="M352" s="0">
-        <v>1168.986</v>
-      </c>
-      <c r="N352" s="0">
-        <v>336.9842</v>
-      </c>
-      <c r="O352" s="0">
-        <v>239.0119</v>
-      </c>
-      <c r="P352" s="0">
-        <v>246.553</v>
-      </c>
-      <c r="Q352" s="0">
-        <v>274.2956</v>
-      </c>
-      <c r="R352" s="0">
-        <v>176.6118</v>
-      </c>
-      <c r="S352" s="0">
-        <v>337.2454</v>
-      </c>
-      <c r="T352" s="0">
-        <v>344.6773</v>
-      </c>
-      <c r="U352" s="0">
-        <v>365.4763</v>
-      </c>
-      <c r="V352" s="0">
-        <v>286.993</v>
-      </c>
-      <c r="W352" s="0">
-        <v>120.3659</v>
-      </c>
-      <c r="X352" s="0">
-        <v>227.6346</v>
-      </c>
-      <c r="Y352" s="0">
-        <v>707.9057</v>
-      </c>
-      <c r="Z352" s="0">
-        <v>505.2217</v>
-      </c>
-      <c r="AA352" s="0">
-        <v>242.9378</v>
-      </c>
-      <c r="AB352" s="0">
-        <v>184.1793</v>
-      </c>
-      <c r="AC352" s="0">
-        <v>133.5248</v>
-      </c>
-      <c r="AD352" s="0">
-        <v>681.9211</v>
-      </c>
-      <c r="AE352" s="0">
-        <v>532.7346</v>
-      </c>
-      <c r="AF352" s="0">
-        <v>416.7398</v>
-      </c>
-      <c r="AG352" s="0">
-        <v>170.6279</v>
-      </c>
-      <c r="AH352" s="0">
-        <v>345.1766</v>
-      </c>
-      <c r="AI352" s="0">
-        <v>1433.597</v>
-      </c>
-      <c r="AJ352" s="0">
-        <v>1367.684</v>
-      </c>
-      <c r="AK352" s="0">
-        <v>889.1747</v>
-      </c>
-      <c r="AL352" s="0">
-        <v>652.5254</v>
-      </c>
-      <c r="AM352" s="0">
-        <v>1150.736</v>
-      </c>
-      <c r="AN352" s="0">
-        <v>179.8613</v>
-      </c>
-      <c r="AO352" s="0">
-        <v>339.8997</v>
-      </c>
-      <c r="AP352" s="0">
-        <v>255.8835</v>
-      </c>
-      <c r="AQ352" s="0">
-        <v>121.2634</v>
-      </c>
-      <c r="AR352" s="0">
-        <v>110.7458</v>
-      </c>
-      <c r="AS352" s="0">
-        <v>742.8247</v>
-      </c>
-      <c r="AT352" s="0">
-        <v>787.1444</v>
-      </c>
-      <c r="AU352" s="0">
-        <v>429.6686</v>
-      </c>
-      <c r="AV352" s="0">
-        <v>877.8477</v>
-      </c>
-      <c r="AW352" s="0">
-        <v>239.5678</v>
-      </c>
-      <c r="AX352" s="0">
-        <v>719.9685</v>
-      </c>
-    </row>
-    <row r="353">
-      <c r="A353" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="B353" s="0">
-        <v>279.8601</v>
-      </c>
-      <c r="C353" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D353" s="0">
-        <v>110.4714</v>
-      </c>
-      <c r="E353" s="0">
-        <v>165.7369</v>
-      </c>
-      <c r="F353" s="0">
-        <v>1254.613</v>
-      </c>
-      <c r="G353" s="0">
-        <v>367.407</v>
-      </c>
-      <c r="H353" s="0">
-        <v>496.9611</v>
-      </c>
-      <c r="I353" s="0">
-        <v>276.2453</v>
-      </c>
-      <c r="J353" s="0">
-        <v>623.5249</v>
-      </c>
-      <c r="K353" s="0">
-        <v>813.7693</v>
-      </c>
-      <c r="L353" s="0">
-        <v>468.5678</v>
-      </c>
-      <c r="M353" s="0">
-        <v>1209.773</v>
-      </c>
-      <c r="N353" s="0">
-        <v>344.9839</v>
-      </c>
-      <c r="O353" s="0">
-        <v>238.9236</v>
-      </c>
-      <c r="P353" s="0">
-        <v>248.9569</v>
-      </c>
-      <c r="Q353" s="0">
-        <v>280.2297</v>
-      </c>
-      <c r="R353" s="0">
-        <v>177.7601</v>
-      </c>
-      <c r="S353" s="0">
-        <v>339.0826</v>
-      </c>
-      <c r="T353" s="0">
-        <v>348.9944</v>
-      </c>
-      <c r="U353" s="0">
-        <v>369.3047</v>
-      </c>
-      <c r="V353" s="0">
-        <v>289.055</v>
-      </c>
-      <c r="W353" s="0">
-        <v>122.881</v>
-      </c>
-      <c r="X353" s="0">
-        <v>229.2457</v>
-      </c>
-      <c r="Y353" s="0">
-        <v>714.5419</v>
-      </c>
-      <c r="Z353" s="0">
-        <v>491.4299</v>
-      </c>
-      <c r="AA353" s="0">
-        <v>246.7487</v>
-      </c>
-      <c r="AB353" s="0">
-        <v>185.1006</v>
-      </c>
-      <c r="AC353" s="0">
-        <v>134.4023</v>
-      </c>
-      <c r="AD353" s="0">
-        <v>694.5627</v>
-      </c>
-      <c r="AE353" s="0">
-        <v>536.0566</v>
-      </c>
-      <c r="AF353" s="0">
-        <v>420.631</v>
-      </c>
-      <c r="AG353" s="0">
-        <v>174.9248</v>
-      </c>
-      <c r="AH353" s="0">
-        <v>348.533</v>
-      </c>
-      <c r="AI353" s="0">
-        <v>1454.22</v>
-      </c>
-      <c r="AJ353" s="0">
-        <v>1390.065</v>
-      </c>
-      <c r="AK353" s="0">
-        <v>896.3394</v>
-      </c>
-      <c r="AL353" s="0">
-        <v>655.914</v>
-      </c>
-      <c r="AM353" s="0">
-        <v>1166.066</v>
-      </c>
-      <c r="AN353" s="0">
-        <v>183.1753</v>
-      </c>
-      <c r="AO353" s="0">
-        <v>346.1908</v>
-      </c>
-      <c r="AP353" s="0">
-        <v>256.8339</v>
-      </c>
-      <c r="AQ353" s="0">
-        <v>124.7598</v>
-      </c>
-      <c r="AR353" s="0">
-        <v>109.0329</v>
-      </c>
-      <c r="AS353" s="0">
-        <v>733.2211</v>
-      </c>
-      <c r="AT353" s="0">
-        <v>812.8061</v>
-      </c>
-      <c r="AU353" s="0">
-        <v>435.9299</v>
-      </c>
-      <c r="AV353" s="0">
-        <v>840.0573</v>
-      </c>
-      <c r="AW353" s="0">
-        <v>240.4808</v>
-      </c>
-      <c r="AX353" s="0">
-        <v>723.6929</v>
-      </c>
-    </row>
-    <row r="354">
-      <c r="A354" s="0" t="s">
-        <v>402</v>
-      </c>
-      <c r="B354" s="0">
-        <v>268.7706</v>
-      </c>
-      <c r="C354" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D354" s="0">
-        <v>112.0909</v>
-      </c>
-      <c r="E354" s="0">
-        <v>167.2994</v>
-      </c>
-      <c r="F354" s="0">
-        <v>1260.828</v>
-      </c>
-      <c r="G354" s="0">
-        <v>372.0729</v>
-      </c>
-      <c r="H354" s="0">
-        <v>500.8201</v>
-      </c>
-      <c r="I354" s="0">
-        <v>279.0848</v>
-      </c>
-      <c r="J354" s="0">
-        <v>634.776</v>
-      </c>
-      <c r="K354" s="0">
-        <v>821.6129</v>
-      </c>
-      <c r="L354" s="0">
-        <v>475.122</v>
-      </c>
-      <c r="M354" s="0">
-        <v>1256.011</v>
-      </c>
-      <c r="N354" s="0">
-        <v>347.8942</v>
-      </c>
-      <c r="O354" s="0">
-        <v>242.7574</v>
-      </c>
-      <c r="P354" s="0">
-        <v>251.0571</v>
-      </c>
-      <c r="Q354" s="0">
-        <v>286.5502</v>
-      </c>
-      <c r="R354" s="0">
-        <v>179.3477</v>
-      </c>
-      <c r="S354" s="0">
-        <v>342.9746</v>
-      </c>
-      <c r="T354" s="0">
-        <v>354.7595</v>
-      </c>
-      <c r="U354" s="0">
-        <v>374.0917</v>
-      </c>
-      <c r="V354" s="0">
-        <v>292.9638</v>
-      </c>
-      <c r="W354" s="0">
-        <v>122.6004</v>
-      </c>
-      <c r="X354" s="0">
-        <v>232.4711</v>
-      </c>
-      <c r="Y354" s="0">
-        <v>721.1083</v>
-      </c>
-      <c r="Z354" s="0">
-        <v>503.7853</v>
-      </c>
-      <c r="AA354" s="0">
-        <v>251.3363</v>
-      </c>
-      <c r="AB354" s="0">
-        <v>186.0544</v>
-      </c>
-      <c r="AC354" s="0">
-        <v>136.0763</v>
-      </c>
-      <c r="AD354" s="0">
-        <v>708.6161</v>
-      </c>
-      <c r="AE354" s="0">
-        <v>544.4605</v>
-      </c>
-      <c r="AF354" s="0">
-        <v>424.1242</v>
-      </c>
-      <c r="AG354" s="0">
-        <v>177.0521</v>
-      </c>
-      <c r="AH354" s="0">
-        <v>356.4313</v>
-      </c>
-      <c r="AI354" s="0">
-        <v>1478.328</v>
-      </c>
-      <c r="AJ354" s="0">
-        <v>1419.04</v>
-      </c>
-      <c r="AK354" s="0">
-        <v>909.3681</v>
-      </c>
-      <c r="AL354" s="0">
-        <v>661.2716</v>
-      </c>
-      <c r="AM354" s="0">
-        <v>1182.003</v>
-      </c>
-      <c r="AN354" s="0">
-        <v>188.0086</v>
-      </c>
-      <c r="AO354" s="0">
-        <v>348.4094</v>
-      </c>
-      <c r="AP354" s="0">
-        <v>258.8672</v>
-      </c>
-      <c r="AQ354" s="0">
-        <v>127.3958</v>
-      </c>
-      <c r="AR354" s="0">
-        <v>113.8729</v>
-      </c>
-      <c r="AS354" s="0">
-        <v>717.5901</v>
-      </c>
-      <c r="AT354" s="0">
-        <v>834.3677</v>
-      </c>
-      <c r="AU354" s="0">
-        <v>441.9744</v>
-      </c>
-      <c r="AV354" s="0">
-        <v>818.1374</v>
-      </c>
-      <c r="AW354" s="0">
-        <v>241.8371</v>
-      </c>
-      <c r="AX354" s="0">
-        <v>733.9572</v>
-      </c>
-    </row>
-    <row r="355">
-      <c r="A355" s="0" t="s">
-        <v>403</v>
-      </c>
-      <c r="B355" s="0">
-        <v>260.3132</v>
-      </c>
-      <c r="C355" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D355" s="0">
-        <v>112.8981</v>
-      </c>
-      <c r="E355" s="0">
-        <v>176.0736</v>
-      </c>
-      <c r="F355" s="0">
-        <v>1271.884</v>
-      </c>
-      <c r="G355" s="0">
-        <v>376.4344</v>
-      </c>
-      <c r="H355" s="0">
-        <v>505.5995</v>
-      </c>
-      <c r="I355" s="0">
-        <v>276.3436</v>
-      </c>
-      <c r="J355" s="0">
-        <v>637.3508</v>
-      </c>
-      <c r="K355" s="0">
-        <v>823.7887</v>
-      </c>
-      <c r="L355" s="0">
-        <v>475.305</v>
-      </c>
-      <c r="M355" s="0">
-        <v>1259.661</v>
-      </c>
-      <c r="N355" s="0">
-        <v>344.2238</v>
-      </c>
-      <c r="O355" s="0">
-        <v>243.6254</v>
-      </c>
-      <c r="P355" s="0">
-        <v>252.6098</v>
-      </c>
-      <c r="Q355" s="0">
-        <v>285.5384</v>
-      </c>
-      <c r="R355" s="0">
-        <v>180.753</v>
-      </c>
-      <c r="S355" s="0">
-        <v>347.1581</v>
-      </c>
-      <c r="T355" s="0">
-        <v>357.1483</v>
-      </c>
-      <c r="U355" s="0">
-        <v>370.6749</v>
-      </c>
-      <c r="V355" s="0">
-        <v>294.3337</v>
-      </c>
-      <c r="W355" s="0">
-        <v>122.648</v>
-      </c>
-      <c r="X355" s="0">
-        <v>236.734</v>
-      </c>
-      <c r="Y355" s="0">
-        <v>721.2084</v>
-      </c>
-      <c r="Z355" s="0">
-        <v>491.7852</v>
-      </c>
-      <c r="AA355" s="0">
-        <v>246.9432</v>
-      </c>
-      <c r="AB355" s="0">
-        <v>187.1847</v>
-      </c>
-      <c r="AC355" s="0">
-        <v>137.5538</v>
-      </c>
-      <c r="AD355" s="0">
-        <v>711.786</v>
-      </c>
-      <c r="AE355" s="0">
-        <v>545.4012</v>
-      </c>
-      <c r="AF355" s="0">
-        <v>429.4149</v>
-      </c>
-      <c r="AG355" s="0">
-        <v>174.7001</v>
-      </c>
-      <c r="AH355" s="0">
-        <v>357.4664</v>
-      </c>
-      <c r="AI355" s="0">
-        <v>1497.101</v>
-      </c>
-      <c r="AJ355" s="0">
-        <v>1424.889</v>
-      </c>
-      <c r="AK355" s="0">
-        <v>923.2549</v>
-      </c>
-      <c r="AL355" s="0">
-        <v>666.0542</v>
-      </c>
-      <c r="AM355" s="0">
-        <v>1198.723</v>
-      </c>
-      <c r="AN355" s="0">
-        <v>184.8855</v>
-      </c>
-      <c r="AO355" s="0">
-        <v>347.8896</v>
-      </c>
-      <c r="AP355" s="0">
-        <v>260.9707</v>
-      </c>
-      <c r="AQ355" s="0">
-        <v>127.9749</v>
-      </c>
-      <c r="AR355" s="0">
-        <v>113.7915</v>
-      </c>
-      <c r="AS355" s="0">
-        <v>713.4767</v>
-      </c>
-      <c r="AT355" s="0">
-        <v>829.8783</v>
-      </c>
-      <c r="AU355" s="0">
-        <v>445.1589</v>
-      </c>
-      <c r="AV355" s="0">
-        <v>791.2059</v>
-      </c>
-      <c r="AW355" s="0">
-        <v>243.3657</v>
-      </c>
-      <c r="AX355" s="0">
-        <v>737.7321</v>
-      </c>
-    </row>
-    <row r="356">
-      <c r="A356" s="0" t="s">
-        <v>404</v>
-      </c>
-      <c r="B356" s="0">
-        <v>272.8799</v>
-      </c>
-      <c r="C356" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D356" s="0">
-        <v>114.9005</v>
-      </c>
-      <c r="E356" s="0">
-        <v>176.0883</v>
-      </c>
-      <c r="F356" s="0">
-        <v>1313.759</v>
-      </c>
-      <c r="G356" s="0">
-        <v>385.9658</v>
-      </c>
-      <c r="H356" s="0">
-        <v>514.0732</v>
-      </c>
-      <c r="I356" s="0">
-        <v>281.1191</v>
-      </c>
-      <c r="J356" s="0">
-        <v>657.6924</v>
-      </c>
-      <c r="K356" s="0">
-        <v>841.8988</v>
-      </c>
-      <c r="L356" s="0">
-        <v>487.8853</v>
-      </c>
-      <c r="M356" s="0">
-        <v>1279.037</v>
-      </c>
-      <c r="N356" s="0">
-        <v>354.1543</v>
-      </c>
-      <c r="O356" s="0">
-        <v>247.0591</v>
-      </c>
-      <c r="P356" s="0">
-        <v>255.2941</v>
-      </c>
-      <c r="Q356" s="0">
-        <v>291.2163</v>
-      </c>
-      <c r="R356" s="0">
-        <v>183.0649</v>
-      </c>
-      <c r="S356" s="0">
-        <v>353.8687</v>
-      </c>
-      <c r="T356" s="0">
-        <v>367.0401</v>
-      </c>
-      <c r="U356" s="0">
-        <v>375.9618</v>
-      </c>
-      <c r="V356" s="0">
-        <v>298.8142</v>
-      </c>
-      <c r="W356" s="0">
-        <v>126.0144</v>
-      </c>
-      <c r="X356" s="0">
-        <v>242.4179</v>
-      </c>
-      <c r="Y356" s="0">
-        <v>737.3809</v>
-      </c>
-      <c r="Z356" s="0">
-        <v>483.1369</v>
-      </c>
-      <c r="AA356" s="0">
-        <v>250.0523</v>
-      </c>
-      <c r="AB356" s="0">
-        <v>188.4365</v>
-      </c>
-      <c r="AC356" s="0">
-        <v>140.2979</v>
-      </c>
-      <c r="AD356" s="0">
-        <v>718.1698</v>
-      </c>
-      <c r="AE356" s="0">
-        <v>554.22</v>
-      </c>
-      <c r="AF356" s="0">
-        <v>437.7885</v>
-      </c>
-      <c r="AG356" s="0">
-        <v>175.3219</v>
-      </c>
-      <c r="AH356" s="0">
-        <v>359.5097</v>
-      </c>
-      <c r="AI356" s="0">
-        <v>1545.247</v>
-      </c>
-      <c r="AJ356" s="0">
-        <v>1479.539</v>
-      </c>
-      <c r="AK356" s="0">
-        <v>952.0504</v>
-      </c>
-      <c r="AL356" s="0">
-        <v>674.5254</v>
-      </c>
-      <c r="AM356" s="0">
-        <v>1229.346</v>
-      </c>
-      <c r="AN356" s="0">
-        <v>186.6011</v>
-      </c>
-      <c r="AO356" s="0">
-        <v>354.6566</v>
-      </c>
-      <c r="AP356" s="0">
-        <v>263.6426</v>
-      </c>
-      <c r="AQ356" s="0">
-        <v>128.4889</v>
-      </c>
-      <c r="AR356" s="0">
-        <v>114.833</v>
-      </c>
-      <c r="AS356" s="0">
-        <v>731.1907</v>
-      </c>
-      <c r="AT356" s="0">
-        <v>875.8335</v>
-      </c>
-      <c r="AU356" s="0">
-        <v>462.657</v>
-      </c>
-      <c r="AV356" s="0">
-        <v>775.3019</v>
-      </c>
-      <c r="AW356" s="0">
-        <v>245.489</v>
-      </c>
-      <c r="AX356" s="0">
-        <v>756.7062</v>
+        <v>679.8239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>